<commit_message>
Refactor report_generator.py to improve formatting and handling of scalar values
</commit_message>
<xml_diff>
--- a/reports/report.xlsx
+++ b/reports/report.xlsx
@@ -578,7 +578,7 @@
       <c r="E2" s="7" t="inlineStr">
         <is>
           <t>Removed:
-pis</t>
+• pis</t>
         </is>
       </c>
     </row>
@@ -598,7 +598,7 @@
       <c r="E3" s="7" t="inlineStr">
         <is>
           <t xml:space="preserve">Removed:
-</t>
+• </t>
         </is>
       </c>
     </row>
@@ -773,7 +773,7 @@
         <is>
           <t>Removed:
 • xs2a_auth_aspsp:
-  - pis</t>
+  -     pis</t>
         </is>
       </c>
     </row>
@@ -799,7 +799,7 @@
       <c r="E9" s="7" t="inlineStr">
         <is>
           <t>Removed:
-pis</t>
+• pis</t>
         </is>
       </c>
     </row>
@@ -819,7 +819,7 @@
       <c r="E10" s="7" t="inlineStr">
         <is>
           <t xml:space="preserve">Removed:
-</t>
+• </t>
         </is>
       </c>
     </row>
@@ -994,7 +994,7 @@
         <is>
           <t>Removed:
 • xs2a_auth_aspsp:
-  - pis</t>
+  -     pis</t>
         </is>
       </c>
     </row>
@@ -1020,7 +1020,7 @@
       <c r="E16" s="7" t="inlineStr">
         <is>
           <t>Removed:
-pis</t>
+• pis</t>
         </is>
       </c>
     </row>
@@ -1195,7 +1195,7 @@
         <is>
           <t>Removed:
 • xs2a_auth_aspsp:
-  - pis</t>
+  -     pis</t>
         </is>
       </c>
     </row>
@@ -1221,7 +1221,7 @@
       <c r="E22" s="7" t="inlineStr">
         <is>
           <t>Removed:
-pis</t>
+• pis</t>
         </is>
       </c>
     </row>
@@ -1241,7 +1241,7 @@
       <c r="E23" s="7" t="inlineStr">
         <is>
           <t xml:space="preserve">Removed:
-</t>
+• </t>
         </is>
       </c>
     </row>
@@ -1416,7 +1416,7 @@
         <is>
           <t>Removed:
 • xs2a_auth_aspsp:
-  - pis</t>
+  -     pis</t>
         </is>
       </c>
     </row>
@@ -1442,7 +1442,7 @@
       <c r="E29" s="7" t="inlineStr">
         <is>
           <t>Removed:
-pis</t>
+• pis</t>
         </is>
       </c>
     </row>
@@ -1462,7 +1462,7 @@
       <c r="E30" s="7" t="inlineStr">
         <is>
           <t xml:space="preserve">Removed:
-</t>
+• </t>
         </is>
       </c>
     </row>
@@ -1637,7 +1637,7 @@
         <is>
           <t>Removed:
 • xs2a_auth_aspsp:
-  - pis</t>
+  -     pis</t>
         </is>
       </c>
     </row>
@@ -1663,7 +1663,7 @@
       <c r="E36" s="7" t="inlineStr">
         <is>
           <t>Removed:
-pis</t>
+• pis</t>
         </is>
       </c>
     </row>
@@ -1683,7 +1683,7 @@
       <c r="E37" s="7" t="inlineStr">
         <is>
           <t xml:space="preserve">Removed:
-</t>
+• </t>
         </is>
       </c>
     </row>
@@ -1858,7 +1858,7 @@
         <is>
           <t>Removed:
 • xs2a_auth_aspsp:
-  - pis</t>
+  -     pis</t>
         </is>
       </c>
     </row>
@@ -1884,7 +1884,7 @@
       <c r="E43" s="7" t="inlineStr">
         <is>
           <t>Removed:
-pis</t>
+• pis</t>
         </is>
       </c>
     </row>
@@ -2059,7 +2059,7 @@
         <is>
           <t>Removed:
 • xs2a_auth_aspsp:
-  - pis</t>
+  -     pis</t>
         </is>
       </c>
     </row>
@@ -2085,7 +2085,7 @@
       <c r="E49" s="7" t="inlineStr">
         <is>
           <t>Removed:
-pis</t>
+• pis</t>
         </is>
       </c>
     </row>
@@ -2260,7 +2260,7 @@
         <is>
           <t>Removed:
 • xs2a_auth_aspsp:
-  - pis</t>
+  -     pis</t>
         </is>
       </c>
     </row>
@@ -2286,7 +2286,7 @@
       <c r="E55" s="7" t="inlineStr">
         <is>
           <t>Removed:
-pis</t>
+• pis</t>
         </is>
       </c>
     </row>
@@ -2461,7 +2461,7 @@
         <is>
           <t>Removed:
 • xs2a_auth_aspsp:
-  - pis</t>
+  -     pis</t>
         </is>
       </c>
     </row>
@@ -2558,19 +2558,19 @@
   description: 
   operationId: getMultiplePayments
   parameters:
-    $ref: #/parameters/acceptEncodingParam
-    $ref: #/parameters/acceptLanguageParam
-    $ref: #/parameters/acceptCharsetParam
-    $ref: #/parameters/xjwsSignatureParam
-    $ref: #/parameters/xRequestIdParam
-    name: payments
-    in: body
-    description: Payments ID list
-    required: True
-    schema:
-      $ref: #/definitions/PaymentsRequest
+    -       $ref: #/parameters/acceptEncodingParam
+    -       $ref: #/parameters/acceptLanguageParam
+    -       $ref: #/parameters/acceptCharsetParam
+    -       $ref: #/parameters/xjwsSignatureParam
+    -       $ref: #/parameters/xRequestIdParam
+    -       name: payments
+      in: body
+      description: Payments ID list
+      required: True
+      schema:
+        $ref: #/definitions/PaymentsRequest
   tags:
-    - PIS
+    -       PIS
   responses:
     200:
       description: Success
@@ -2644,7 +2644,7 @@
       <c r="E62" s="7" t="inlineStr">
         <is>
           <t>Removed:
-pis</t>
+• pis</t>
         </is>
       </c>
     </row>
@@ -2819,7 +2819,7 @@
         <is>
           <t>Removed:
 • xs2a_auth_aspsp:
-  - pis</t>
+  -     pis</t>
         </is>
       </c>
     </row>
@@ -2845,7 +2845,7 @@
       <c r="E68" s="7" t="inlineStr">
         <is>
           <t>Removed:
-pis</t>
+• pis</t>
         </is>
       </c>
     </row>
@@ -3020,7 +3020,7 @@
         <is>
           <t>Removed:
 • xs2a_auth_aspsp:
-  - pis</t>
+  -     pis</t>
         </is>
       </c>
     </row>
@@ -3118,19 +3118,19 @@
   description: Confirming the availability on the payers account of the amount necessary to execute the payment transaction, as defined in Art. 65 PSD2.
   operationId: getConfirmationOfFunds
   parameters:
-    $ref: #/parameters/acceptEncodingParam
-    $ref: #/parameters/acceptLanguageParam
-    $ref: #/parameters/acceptCharsetParam
-    $ref: #/parameters/xjwsSignatureParam
-    $ref: #/parameters/xRequestIdParam
-    name: confirmationOfFundsRequest
-    in: body
-    description: Object with amount to check
-    required: True
-    schema:
-      $ref: #/definitions/ConfirmationOfFundsRequest
+    -       $ref: #/parameters/acceptEncodingParam
+    -       $ref: #/parameters/acceptLanguageParam
+    -       $ref: #/parameters/acceptCharsetParam
+    -       $ref: #/parameters/xjwsSignatureParam
+    -       $ref: #/parameters/xRequestIdParam
+    -       name: confirmationOfFundsRequest
+      in: body
+      description: Object with amount to check
+      required: True
+      schema:
+        $ref: #/definitions/ConfirmationOfFundsRequest
   tags:
-    - CAF
+    -       CAF
   responses:
     200:
       description: Success
@@ -3270,19 +3270,19 @@
   description: Removes consent
   operationId: deleteConsent
   parameters:
-    $ref: #/parameters/acceptEncodingParam
-    $ref: #/parameters/acceptLanguageParam
-    $ref: #/parameters/acceptCharsetParam
-    $ref: #/parameters/xjwsSignatureParam
-    $ref: #/parameters/xRequestIdParam
-    name: deleteConsentRequest
-    in: body
-    description: Data for delete Consent Request
-    required: True
-    schema:
-      $ref: #/definitions/DeleteConsentRequest
+    -       $ref: #/parameters/acceptEncodingParam
+    -       $ref: #/parameters/acceptLanguageParam
+    -       $ref: #/parameters/acceptCharsetParam
+    -       $ref: #/parameters/xjwsSignatureParam
+    -       $ref: #/parameters/xRequestIdParam
+    -       name: deleteConsentRequest
+      in: body
+      description: Data for delete Consent Request
+      required: True
+      schema:
+        $ref: #/definitions/DeleteConsentRequest
   tags:
-    - AIS
+    -       AIS
   responses:
     204:
       description: Success
@@ -3432,20 +3432,20 @@
   description: User identification based on access token
   operationId: getAccounts
   parameters:
-    $ref: #/parameters/authorizationParam
-    $ref: #/parameters/acceptEncodingParam
-    $ref: #/parameters/acceptLanguageParam
-    $ref: #/parameters/acceptCharsetParam
-    $ref: #/parameters/xjwsSignatureParam
-    $ref: #/parameters/xRequestIdParam
-    name: getAccountsRequest
-    in: body
-    description: Data for Accounts Request
-    required: True
-    schema:
-      $ref: #/definitions/AccountsRequest
+    -       $ref: #/parameters/authorizationParam
+    -       $ref: #/parameters/acceptEncodingParam
+    -       $ref: #/parameters/acceptLanguageParam
+    -       $ref: #/parameters/acceptCharsetParam
+    -       $ref: #/parameters/xjwsSignatureParam
+    -       $ref: #/parameters/xRequestIdParam
+    -       name: getAccountsRequest
+      in: body
+      description: Data for Accounts Request
+      required: True
+      schema:
+        $ref: #/definitions/AccountsRequest
   tags:
-    - AIS
+    -       AIS
   responses:
     200:
       description: Success
@@ -3499,10 +3499,10 @@
       schema:
         $ref: #/definitions/Error
   security:
-    xs2a_auth_aspsp:
-      - ais-accounts
-    xs2a_auth_decoupled:
-      - ais-accounts</t>
+    -       xs2a_auth_aspsp:
+        -           ais-accounts
+    -       xs2a_auth_decoupled:
+        -           ais-accounts</t>
         </is>
       </c>
     </row>
@@ -3609,20 +3609,20 @@
   description: User identification based on access token
   operationId: getAccount
   parameters:
-    $ref: #/parameters/authorizationParam
-    $ref: #/parameters/acceptEncodingParam
-    $ref: #/parameters/acceptLanguageParam
-    $ref: #/parameters/acceptCharsetParam
-    $ref: #/parameters/xjwsSignatureParam
-    $ref: #/parameters/xRequestIdParam
-    name: getAccountRequest
-    in: body
-    description: Data for Account Request
-    required: True
-    schema:
-      $ref: #/definitions/AccountInfoRequest
+    -       $ref: #/parameters/authorizationParam
+    -       $ref: #/parameters/acceptEncodingParam
+    -       $ref: #/parameters/acceptLanguageParam
+    -       $ref: #/parameters/acceptCharsetParam
+    -       $ref: #/parameters/xjwsSignatureParam
+    -       $ref: #/parameters/xRequestIdParam
+    -       name: getAccountRequest
+      in: body
+      description: Data for Account Request
+      required: True
+      schema:
+        $ref: #/definitions/AccountInfoRequest
   tags:
-    - AIS
+    -       AIS
   responses:
     200:
       description: Success
@@ -3676,10 +3676,10 @@
       schema:
         $ref: #/definitions/Error
   security:
-    xs2a_auth_aspsp:
-      - ais
-    xs2a_auth_decoupled:
-      - ais</t>
+    -       xs2a_auth_aspsp:
+        -           ais
+    -       xs2a_auth_decoupled:
+        -           ais</t>
         </is>
       </c>
     </row>
@@ -3786,20 +3786,20 @@
   description: 
   operationId: getTransactionsDone
   parameters:
-    $ref: #/parameters/authorizationParam
-    $ref: #/parameters/acceptEncodingParam
-    $ref: #/parameters/acceptLanguageParam
-    $ref: #/parameters/acceptCharsetParam
-    $ref: #/parameters/xjwsSignatureParam
-    $ref: #/parameters/xRequestIdParam
-    name: getTransactionsDoneRequest
-    in: body
-    description: Data for Transactions Done Request
-    required: True
-    schema:
-      $ref: #/definitions/TransactionInfoRequest
+    -       $ref: #/parameters/authorizationParam
+    -       $ref: #/parameters/acceptEncodingParam
+    -       $ref: #/parameters/acceptLanguageParam
+    -       $ref: #/parameters/acceptCharsetParam
+    -       $ref: #/parameters/xjwsSignatureParam
+    -       $ref: #/parameters/xRequestIdParam
+    -       name: getTransactionsDoneRequest
+      in: body
+      description: Data for Transactions Done Request
+      required: True
+      schema:
+        $ref: #/definitions/TransactionInfoRequest
   tags:
-    - AIS
+    -       AIS
   responses:
     200:
       description: Success
@@ -3853,10 +3853,10 @@
       schema:
         $ref: #/definitions/Error
   security:
-    xs2a_auth_aspsp:
-      - ais
-    xs2a_auth_decoupled:
-      - ais</t>
+    -       xs2a_auth_aspsp:
+        -           ais
+    -       xs2a_auth_decoupled:
+        -           ais</t>
         </is>
       </c>
     </row>
@@ -3963,20 +3963,20 @@
   description: 
   operationId: getTransactionsPending
   parameters:
-    $ref: #/parameters/authorizationParam
-    $ref: #/parameters/acceptEncodingParam
-    $ref: #/parameters/acceptLanguageParam
-    $ref: #/parameters/acceptCharsetParam
-    $ref: #/parameters/xjwsSignatureParam
-    $ref: #/parameters/xRequestIdParam
-    name: getTransactionsPendingRequest
-    in: body
-    description: Data for Transactions Pending Request
-    required: True
-    schema:
-      $ref: #/definitions/TransactionInfoRequest
+    -       $ref: #/parameters/authorizationParam
+    -       $ref: #/parameters/acceptEncodingParam
+    -       $ref: #/parameters/acceptLanguageParam
+    -       $ref: #/parameters/acceptCharsetParam
+    -       $ref: #/parameters/xjwsSignatureParam
+    -       $ref: #/parameters/xRequestIdParam
+    -       name: getTransactionsPendingRequest
+      in: body
+      description: Data for Transactions Pending Request
+      required: True
+      schema:
+        $ref: #/definitions/TransactionInfoRequest
   tags:
-    - AIS
+    -       AIS
   responses:
     200:
       description: Success
@@ -4030,10 +4030,10 @@
       schema:
         $ref: #/definitions/Error
   security:
-    xs2a_auth_aspsp:
-      - ais
-    xs2a_auth_decoupled:
-      - ais</t>
+    -       xs2a_auth_aspsp:
+        -           ais
+    -       xs2a_auth_decoupled:
+        -           ais</t>
         </is>
       </c>
     </row>
@@ -4140,20 +4140,20 @@
   description: 
   operationId: getTransactionsRejected
   parameters:
-    $ref: #/parameters/authorizationParam
-    $ref: #/parameters/acceptEncodingParam
-    $ref: #/parameters/acceptLanguageParam
-    $ref: #/parameters/acceptCharsetParam
-    $ref: #/parameters/xjwsSignatureParam
-    $ref: #/parameters/xRequestIdParam
-    name: getTransactionsRejectedRequest
-    in: body
-    description: Data for Transactions Rejected Request
-    required: True
-    schema:
-      $ref: #/definitions/TransactionInfoRequest
+    -       $ref: #/parameters/authorizationParam
+    -       $ref: #/parameters/acceptEncodingParam
+    -       $ref: #/parameters/acceptLanguageParam
+    -       $ref: #/parameters/acceptCharsetParam
+    -       $ref: #/parameters/xjwsSignatureParam
+    -       $ref: #/parameters/xRequestIdParam
+    -       name: getTransactionsRejectedRequest
+      in: body
+      description: Data for Transactions Rejected Request
+      required: True
+      schema:
+        $ref: #/definitions/TransactionInfoRequest
   tags:
-    - AIS
+    -       AIS
   responses:
     200:
       description: Success
@@ -4207,10 +4207,10 @@
       schema:
         $ref: #/definitions/Error
   security:
-    xs2a_auth_aspsp:
-      - ais
-    xs2a_auth_decoupled:
-      - ais</t>
+    -       xs2a_auth_aspsp:
+        -           ais
+    -       xs2a_auth_decoupled:
+        -           ais</t>
         </is>
       </c>
     </row>
@@ -4317,20 +4317,20 @@
   description: 
   operationId: getTransactionsCancelled
   parameters:
-    $ref: #/parameters/authorizationParam
-    $ref: #/parameters/acceptEncodingParam
-    $ref: #/parameters/acceptLanguageParam
-    $ref: #/parameters/acceptCharsetParam
-    $ref: #/parameters/xjwsSignatureParam
-    $ref: #/parameters/xRequestIdParam
-    name: getTransactionsCancelledRequest
-    in: body
-    description: Data for Transactions Cancelled Request
-    required: True
-    schema:
-      $ref: #/definitions/TransactionInfoRequest
+    -       $ref: #/parameters/authorizationParam
+    -       $ref: #/parameters/acceptEncodingParam
+    -       $ref: #/parameters/acceptLanguageParam
+    -       $ref: #/parameters/acceptCharsetParam
+    -       $ref: #/parameters/xjwsSignatureParam
+    -       $ref: #/parameters/xRequestIdParam
+    -       name: getTransactionsCancelledRequest
+      in: body
+      description: Data for Transactions Cancelled Request
+      required: True
+      schema:
+        $ref: #/definitions/TransactionInfoRequest
   tags:
-    - AIS
+    -       AIS
   responses:
     200:
       description: Success
@@ -4384,10 +4384,10 @@
       schema:
         $ref: #/definitions/Error
   security:
-    xs2a_auth_aspsp:
-      - ais
-    xs2a_auth_decoupled:
-      - ais</t>
+    -       xs2a_auth_aspsp:
+        -           ais
+    -       xs2a_auth_decoupled:
+        -           ais</t>
         </is>
       </c>
     </row>
@@ -4494,20 +4494,20 @@
   description: 
   operationId: getTransactionsScheduled
   parameters:
-    $ref: #/parameters/authorizationParam
-    $ref: #/parameters/acceptEncodingParam
-    $ref: #/parameters/acceptLanguageParam
-    $ref: #/parameters/acceptCharsetParam
-    $ref: #/parameters/xjwsSignatureParam
-    $ref: #/parameters/xRequestIdParam
-    name: getTransactionsScheduledRequest
-    in: body
-    description: Data for Transactions Scheduled Request
-    required: True
-    schema:
-      $ref: #/definitions/TransactionInfoRequest
+    -       $ref: #/parameters/authorizationParam
+    -       $ref: #/parameters/acceptEncodingParam
+    -       $ref: #/parameters/acceptLanguageParam
+    -       $ref: #/parameters/acceptCharsetParam
+    -       $ref: #/parameters/xjwsSignatureParam
+    -       $ref: #/parameters/xRequestIdParam
+    -       name: getTransactionsScheduledRequest
+      in: body
+      description: Data for Transactions Scheduled Request
+      required: True
+      schema:
+        $ref: #/definitions/TransactionInfoRequest
   tags:
-    - AIS
+    -       AIS
   responses:
     200:
       description: Success
@@ -4561,10 +4561,10 @@
       schema:
         $ref: #/definitions/Error
   security:
-    xs2a_auth_aspsp:
-      - ais
-    xs2a_auth_decoupled:
-      - ais</t>
+    -       xs2a_auth_aspsp:
+        -           ais
+    -       xs2a_auth_decoupled:
+        -           ais</t>
         </is>
       </c>
     </row>
@@ -4671,20 +4671,20 @@
   description: 
   operationId: getHolds
   parameters:
-    $ref: #/parameters/authorizationParam
-    $ref: #/parameters/acceptEncodingParam
-    $ref: #/parameters/acceptLanguageParam
-    $ref: #/parameters/acceptCharsetParam
-    $ref: #/parameters/xjwsSignatureParam
-    $ref: #/parameters/xRequestIdParam
-    name: getHoldsRequest
-    in: body
-    description: Data for hold Request
-    required: True
-    schema:
-      $ref: #/definitions/HoldRequest
+    -       $ref: #/parameters/authorizationParam
+    -       $ref: #/parameters/acceptEncodingParam
+    -       $ref: #/parameters/acceptLanguageParam
+    -       $ref: #/parameters/acceptCharsetParam
+    -       $ref: #/parameters/xjwsSignatureParam
+    -       $ref: #/parameters/xRequestIdParam
+    -       name: getHoldsRequest
+      in: body
+      description: Data for hold Request
+      required: True
+      schema:
+        $ref: #/definitions/HoldRequest
   tags:
-    - AIS
+    -       AIS
   responses:
     200:
       description: Success
@@ -4738,10 +4738,10 @@
       schema:
         $ref: #/definitions/Error
   security:
-    xs2a_auth_aspsp:
-      - ais
-    xs2a_auth_decoupled:
-      - ais</t>
+    -       xs2a_auth_aspsp:
+        -           ais
+    -       xs2a_auth_decoupled:
+        -           ais</t>
         </is>
       </c>
     </row>
@@ -4848,20 +4848,20 @@
   description: 
   operationId: getTransactionDetail
   parameters:
-    $ref: #/parameters/authorizationParam
-    $ref: #/parameters/acceptEncodingParam
-    $ref: #/parameters/acceptLanguageParam
-    $ref: #/parameters/acceptCharsetParam
-    $ref: #/parameters/xjwsSignatureParam
-    $ref: #/parameters/xRequestIdParam
-    name: getTransationDetailRequest
-    in: body
-    description: Data for transation detail Request
-    required: True
-    schema:
-      $ref: #/definitions/TransactionDetailRequest
+    -       $ref: #/parameters/authorizationParam
+    -       $ref: #/parameters/acceptEncodingParam
+    -       $ref: #/parameters/acceptLanguageParam
+    -       $ref: #/parameters/acceptCharsetParam
+    -       $ref: #/parameters/xjwsSignatureParam
+    -       $ref: #/parameters/xRequestIdParam
+    -       name: getTransationDetailRequest
+      in: body
+      description: Data for transation detail Request
+      required: True
+      schema:
+        $ref: #/definitions/TransactionDetailRequest
   tags:
-    - AIS
+    -       AIS
   responses:
     200:
       description: Success
@@ -4915,10 +4915,10 @@
       schema:
         $ref: #/definitions/Error
   security:
-    xs2a_auth_aspsp:
-      - ais
-    xs2a_auth_decoupled:
-      - ais</t>
+    -       xs2a_auth_aspsp:
+        -           ais
+    -       xs2a_auth_decoupled:
+        -           ais</t>
         </is>
       </c>
     </row>
@@ -5007,19 +5007,19 @@
   description: Requests OAuth2 authorization code
   operationId: authorize
   parameters:
-    $ref: #/parameters/acceptEncodingParam
-    $ref: #/parameters/acceptLanguageParam
-    $ref: #/parameters/acceptCharsetParam
-    $ref: #/parameters/xjwsSignatureParam
-    $ref: #/parameters/xRequestIdParam
-    name: authorizeRequest
-    in: body
-    description: Data for OAuth2 Authorization Code Request
-    required: True
-    schema:
-      $ref: #/definitions/AuthorizeRequest
+    -       $ref: #/parameters/acceptEncodingParam
+    -       $ref: #/parameters/acceptLanguageParam
+    -       $ref: #/parameters/acceptCharsetParam
+    -       $ref: #/parameters/xjwsSignatureParam
+    -       $ref: #/parameters/xRequestIdParam
+    -       name: authorizeRequest
+      in: body
+      description: Data for OAuth2 Authorization Code Request
+      required: True
+      schema:
+        $ref: #/definitions/AuthorizeRequest
   tags:
-    - AS
+    -       AS
   responses:
     200:
       description: Success
@@ -5149,19 +5149,19 @@
   description: Requests OAuth2 authorization code based One-time authorization code issued by External Authorization Tool. Authorization code will be delivered to TPP as callback request from ASPSP if PSU authentication is confirmed by EAT. Callback function must provide similar notification also in case of unsuccessful authentication or its abandonment.
   operationId: authorizeExt
   parameters:
-    $ref: #/parameters/acceptEncodingParam
-    $ref: #/parameters/acceptLanguageParam
-    $ref: #/parameters/acceptCharsetParam
-    $ref: #/parameters/xjwsSignatureParam
-    $ref: #/parameters/xRequestIdParam
-    name: eatCodeRequest
-    in: body
-    description: Data for OAuth2 Authorization Code Request extended for EAT based authentication and callback response
-    required: True
-    schema:
-      $ref: #/definitions/EatCodeRequest
+    -       $ref: #/parameters/acceptEncodingParam
+    -       $ref: #/parameters/acceptLanguageParam
+    -       $ref: #/parameters/acceptCharsetParam
+    -       $ref: #/parameters/xjwsSignatureParam
+    -       $ref: #/parameters/xRequestIdParam
+    -       name: eatCodeRequest
+      in: body
+      description: Data for OAuth2 Authorization Code Request extended for EAT based authentication and callback response
+      required: True
+      schema:
+        $ref: #/definitions/EatCodeRequest
   tags:
-    - AS
+    -       AS
   responses:
     204:
       description: Successful TPP and EAT Code verification
@@ -5289,19 +5289,19 @@
   description: Requests OAuth2 access token value
   operationId: token
   parameters:
-    $ref: #/parameters/acceptEncodingParam
-    $ref: #/parameters/acceptLanguageParam
-    $ref: #/parameters/acceptCharsetParam
-    $ref: #/parameters/xjwsSignatureParam
-    $ref: #/parameters/xRequestIdParam
-    name: tokenRequest
-    in: body
-    description: Data for OAuth2 Access Token Request
-    required: True
-    schema:
-      $ref: #/definitions/TokenRequest
+    -       $ref: #/parameters/acceptEncodingParam
+    -       $ref: #/parameters/acceptLanguageParam
+    -       $ref: #/parameters/acceptCharsetParam
+    -       $ref: #/parameters/xjwsSignatureParam
+    -       $ref: #/parameters/xRequestIdParam
+    -       name: tokenRequest
+      in: body
+      description: Data for OAuth2 Access Token Request
+      required: True
+      schema:
+        $ref: #/definitions/TokenRequest
   tags:
-    - AS
+    -       AS
   responses:
     200:
       description: Success
@@ -5407,13 +5407,13 @@
 • description: Klasa zapytania o uzyskanie kodu autoryzacyjnego zgodnego z OAuth2
 • type: object
 • required:
-  - requestHeader
-  - response_type
-  - client_id
-  - redirect_uri
-  - scope
-  - scope_details
-  - state
+  -     requestHeader
+  -     response_type
+  -     client_id
+  -     redirect_uri
+  -     scope
+  -     scope_details
+  -     state
 • properties:
   requestHeader:
     $ref: #/definitions/RequestHeaderWithoutTokenAS
@@ -5475,8 +5475,8 @@
           <t>Removed:
 • description: Klasa odpowiedzi na zapytanie TPP o autoryzację PSU do wykonania usługi interfejsu XS2A
 • required:
-  - responseHeader
-  - aspspRedirectUri
+  -     responseHeader
+  -     aspspRedirectUri
 • properties:
   responseHeader:
     $ref: #/definitions/ResponseHeader
@@ -5550,15 +5550,15 @@
 • description: Klasa zapytania o uzyskanie kodu autoryzacyjnego zgodnego z OAuth2 na podstawie przekazanego kodu jednorazowego, wygenerowanego w EAT
 • type: object
 • required:
-  - requestHeader
-  - requestId
-  - response_type
-  - eatCode
-  - client_id
-  - callbackURL
-  - apiKey
-  - scope
-  - scope_details
+  -     requestHeader
+  -     requestId
+  -     response_type
+  -     eatCode
+  -     client_id
+  -     callbackURL
+  -     apiKey
+  -     scope
+  -     scope_details
 • properties:
   requestHeader:
     $ref: #/definitions/RequestHeaderWithoutTokenCallbackAS
@@ -5665,7 +5665,7 @@
 • description: Klasa zapytania o uzyskanie tokena dostępowego zgodnego z OAuth2
 • type: object
 • required:
-  - grant_type
+  -     grant_type
 • properties:
   requestHeader:
     $ref: #/definitions/RequestHeaderWithoutTokenAS
@@ -5761,11 +5761,11 @@
           <t>Removed:
 • description: Klasa odpowiedzi na zapytanie TPP o wygenerowanie tokena dostępowego
 • required:
-  - responseHeader
-  - access_token
-  - token_type
-  - expires_in
-  - scope_details
+  -     responseHeader
+  -     access_token
+  -     token_type
+  -     expires_in
+  -     scope_details
 • properties:
   responseHeader:
     $ref: #/definitions/ResponseHeader
@@ -5822,7 +5822,7 @@
 • description: Klasa zapytania o usunięcie zgody na dostęp do AIS
 • type: object
 • required:
-  - consentId
+  -     consentId
 • properties:
   consentId:
     type: string
@@ -5875,7 +5875,7 @@
 • description: Klasa zapytania o rachunki / Accounts Request Class
 • type: object
 • required:
-  - requestHeader
+  -     requestHeader
 • properties:
   requestHeader:
     $ref: #/definitions/RequestHeaderAISCallback
@@ -5922,7 +5922,7 @@
           <t>Removed:
 • description: Klasa odpowiedzi na zapytania o konto PSU / PSU's Account Response Class
 • required:
-  - responseHeader
+  -     responseHeader
 • properties:
   responseHeader:
     $ref: #/definitions/ResponseHeader
@@ -5966,7 +5966,7 @@
           <t>Removed:
 • description: Klasa odpowiedzi na zapytania o wiele kont PSU / PSU's Multiple Accounts Response Class
 • required:
-  - responseHeader
+  -     responseHeader
 • properties:
   responseHeader:
     $ref: #/definitions/ResponseHeader
@@ -6022,9 +6022,9 @@
 • description: Klasa informacji o koncie / Account Information Class
 • type: object
 • required:
-  - accountNumber
-  - accountTypeName
-  - accountType
+  -     accountNumber
+  -     accountTypeName
+  -     accountType
 • properties:
   accountNumber:
     type: string
@@ -6117,13 +6117,13 @@
 • description: Klasa informacji o koncie / Account Information Class
 • type: object
 • required:
-  - accountNumber
-  - nameAddress
-  - availableBalance
-  - bookingBalance
-  - currency
-  - accountType
-  - accountHolderType
+  -     accountNumber
+  -     nameAddress
+  -     availableBalance
+  -     bookingBalance
+  -     currency
+  -     accountType
+  -     accountHolderType
 • properties:
   accountNumber:
     type: string
@@ -6139,8 +6139,8 @@
   accountHolderType:
     type: string
     enum:
-      - individual
-      - corporation
+      -         individual
+      -         corporation
     description: Rodzaj posiadacza rachunku: osoba fizyczna lub osoba prawna / Account holder type: individual person or corporation
   accountNameClient:
     type: string
@@ -6203,8 +6203,8 @@
 • description: Klasa zapytania o pojedynczy rachunek / Account Information Request Class
 • type: object
 • required:
-  - requestHeader
-  - accountNumber
+  -     requestHeader
+  -     accountNumber
 • properties:
   requestHeader:
     $ref: #/definitions/RequestHeaderAIS
@@ -6386,18 +6386,18 @@
           <t>Removed:
 • description: Klasa zapytania o transakcje / Transaction Information Request Class
 • allOf:
-  $ref: #/definitions/ItemInfoRequestBase
-  type: object
-  required:
-    - requestHeader
-    - accountNumber
-  properties:
-    type:
-      type: string
-      enum:
-        - CREDIT
-        - DEBIT
-      description: Element filtru: transakcji / Filter element
+  -     $ref: #/definitions/ItemInfoRequestBase
+  -     type: object
+    required:
+      -         requestHeader
+      -         accountNumber
+    properties:
+      type:
+        type: string
+        enum:
+          -             CREDIT
+          -             DEBIT
+        description: Element filtru: transakcji / Filter element
 • xml:
   name: TransactionInfoRequest</t>
         </is>
@@ -6441,17 +6441,17 @@
           <t>Removed:
 • description: Klasa zapytania o elementy (transakcje lub blokady) / Element (transaction or hold) Information Request Class
 • allOf:
-  $ref: #/definitions/ItemInfoRequestBase
-  type: object
-  required:
-    - requestHeader
-    - accountNumber
-  properties:
-    type:
-      type: string
-      enum:
-        - DEBIT
-      description: Element filtru: transakcji / Filter element
+  -     $ref: #/definitions/ItemInfoRequestBase
+  -     type: object
+    required:
+      -         requestHeader
+      -         accountNumber
+    properties:
+      type:
+        type: string
+        enum:
+          -             DEBIT
+        description: Element filtru: transakcji / Filter element
 • xml:
   name: HoldRequest</t>
         </is>
@@ -6518,8 +6518,8 @@
 • description: Klasa bazowa informacji o elemencie (transakcji lub blokadzie) / Element (transaction or hold) Information Base Class
 • type: object
 • required:
-  - itemId
-  - amount
+  -     itemId
+  -     amount
 • properties:
   itemId:
     type: string
@@ -6595,22 +6595,22 @@
           <t>Removed:
 • description: Klasa opisująca blokadę na rachunku / Hold info class
 • allOf:
-  $ref: #/definitions/ItemInfoBase
-  type: object
-  required:
-    - itemId
-    - amount
-  properties:
-    holdExpirationDate:
-      type: string
-      format: date-time
-      description: Data ważności blokady, YYYY-MM-DDThh:mm:ss[.mmm]
-    initiator:
-      $ref: #/definitions/NameAddress
-    sender:
-      $ref: #/definitions/SenderRecipient
-    recipient:
-      $ref: #/definitions/SenderRecipient
+  -     $ref: #/definitions/ItemInfoBase
+  -     type: object
+    required:
+      -         itemId
+      -         amount
+    properties:
+      holdExpirationDate:
+        type: string
+        format: date-time
+        description: Data ważności blokady, YYYY-MM-DDThh:mm:ss[.mmm]
+      initiator:
+        $ref: #/definitions/NameAddress
+      sender:
+        $ref: #/definitions/SenderRecipient
+      recipient:
+        $ref: #/definitions/SenderRecipient
 • xml:
   name: HoldInfo</t>
         </is>
@@ -6664,25 +6664,25 @@
           <t>Removed:
 • description: Klasa opisująca oczekującą transakcję płatniczą. Jest to transakcja niezaksięgowana, niemodyfikowalna, wpływającej na dostępne środki (saldo dostępne).
 • allOf:
-  $ref: #/definitions/ItemInfoBase
-  type: object
-  required:
-    - itemId
-    - amount
-    - transactionCategory
-  properties:
-    transactionCategory:
-      type: string
-      enum:
-        - CREDIT
-        - DEBIT
-      description: Kategoria transakcji uznanie/obciążenie / Transaction category (credit/debit)
-    initiator:
-      $ref: #/definitions/NameAddress
-    sender:
-      $ref: #/definitions/SenderRecipient
-    recipient:
-      $ref: #/definitions/SenderRecipient
+  -     $ref: #/definitions/ItemInfoBase
+  -     type: object
+    required:
+      -         itemId
+      -         amount
+      -         transactionCategory
+    properties:
+      transactionCategory:
+        type: string
+        enum:
+          -             CREDIT
+          -             DEBIT
+        description: Kategoria transakcji uznanie/obciążenie / Transaction category (credit/debit)
+      initiator:
+        $ref: #/definitions/NameAddress
+      sender:
+        $ref: #/definitions/SenderRecipient
+      recipient:
+        $ref: #/definitions/SenderRecipient
 • xml:
   name: TransactionPendingInfo</t>
         </is>
@@ -6742,33 +6742,33 @@
           <t>Removed:
 • description: Klasa opisująca odrzuconą transakcję płatniczą
 • allOf:
-  $ref: #/definitions/ItemInfoBase
-  type: object
-  required:
-    - itemId
-    - amount
-    - transactionCategory
-  properties:
-    transactionCategory:
-      type: string
-      enum:
-        - CREDIT
-        - DEBIT
-      description: Kategoria transakcji uznanie/obciążenie / Transaction category (credit/debit)
-    initiator:
-      $ref: #/definitions/NameAddress
-    sender:
-      $ref: #/definitions/SenderRecipient
-    recipient:
-      $ref: #/definitions/SenderRecipient
-    rejectionReason:
-      type: string
-      maxLength: 140
-      description: Powod odrzucenia
-    rejectionDate:
-      type: string
-      format: date-time
-      description: Data odrzucenia, YYYY-MM-DDThh:mm:ss[.mmm]
+  -     $ref: #/definitions/ItemInfoBase
+  -     type: object
+    required:
+      -         itemId
+      -         amount
+      -         transactionCategory
+    properties:
+      transactionCategory:
+        type: string
+        enum:
+          -             CREDIT
+          -             DEBIT
+        description: Kategoria transakcji uznanie/obciążenie / Transaction category (credit/debit)
+      initiator:
+        $ref: #/definitions/NameAddress
+      sender:
+        $ref: #/definitions/SenderRecipient
+      recipient:
+        $ref: #/definitions/SenderRecipient
+      rejectionReason:
+        type: string
+        maxLength: 140
+        description: Powod odrzucenia
+      rejectionDate:
+        type: string
+        format: date-time
+        description: Data odrzucenia, YYYY-MM-DDThh:mm:ss[.mmm]
 • xml:
   name: TransactionRejectedInfo</t>
         </is>
@@ -6832,35 +6832,35 @@
           <t>Removed:
 • description: Klasa opisująca transakcję płatniczą
 • allOf:
-  $ref: #/definitions/ItemInfoBase
-  type: object
-  required:
-    - itemId
-    - amount
-    - transactionCategory
-  properties:
-    transactionCategory:
-      type: string
-      enum:
-        - CREDIT
-        - DEBIT
-      description: Kategoria transakcji uznanie/obciążenie / Transaction category (credit/debit)
-    transactionStatus:
-      $ref: #/definitions/DictionaryItem
-    initiator:
-      $ref: #/definitions/NameAddress
-    sender:
-      $ref: #/definitions/SenderRecipient
-    recipient:
-      $ref: #/definitions/SenderRecipient
-    bookingDate:
-      type: string
-      format: date-time
-      description: Data księgowania, YYYY-MM-DDThh:mm:ss[.mmm]. Wymagane warunkowo - w przypadku transakcji zaksięgowanych.
-    postTransactionBalance:
-      type: string
-      pattern: ^-?(0|([1-9][0-9]{0,}))\.\d{2}$
-      description: Saldo rachunku po transakcji. Wymagane warunkowo - w przypadku transakcji zaksięgowanych.
+  -     $ref: #/definitions/ItemInfoBase
+  -     type: object
+    required:
+      -         itemId
+      -         amount
+      -         transactionCategory
+    properties:
+      transactionCategory:
+        type: string
+        enum:
+          -             CREDIT
+          -             DEBIT
+        description: Kategoria transakcji uznanie/obciążenie / Transaction category (credit/debit)
+      transactionStatus:
+        $ref: #/definitions/DictionaryItem
+      initiator:
+        $ref: #/definitions/NameAddress
+      sender:
+        $ref: #/definitions/SenderRecipient
+      recipient:
+        $ref: #/definitions/SenderRecipient
+      bookingDate:
+        type: string
+        format: date-time
+        description: Data księgowania, YYYY-MM-DDThh:mm:ss[.mmm]. Wymagane warunkowo - w przypadku transakcji zaksięgowanych.
+      postTransactionBalance:
+        type: string
+        pattern: ^-?(0|([1-9][0-9]{0,}))\.\d{2}$
+        description: Saldo rachunku po transakcji. Wymagane warunkowo - w przypadku transakcji zaksięgowanych.
 • xml:
   name: TransactionInfo</t>
         </is>
@@ -6914,27 +6914,27 @@
           <t>Removed:
 • description: Klasa opisująca odwołaną transakcję płatniczą
 • allOf:
-  $ref: #/definitions/ItemInfoBase
-  type: object
-  required:
-    - itemId
-    - amount
-    - transactionCategory
-  properties:
-    transactionCategory:
-      type: string
-      enum:
-        - CREDIT
-        - DEBIT
-      description: Kategoria transakcji uznanie/obciążenie / Transaction category (credit/debit)
-    transactionStatus:
-      $ref: #/definitions/DictionaryItem
-    initiator:
-      $ref: #/definitions/NameAddress
-    sender:
-      $ref: #/definitions/SenderRecipient
-    recipient:
-      $ref: #/definitions/SenderRecipient
+  -     $ref: #/definitions/ItemInfoBase
+  -     type: object
+    required:
+      -         itemId
+      -         amount
+      -         transactionCategory
+    properties:
+      transactionCategory:
+        type: string
+        enum:
+          -             CREDIT
+          -             DEBIT
+        description: Kategoria transakcji uznanie/obciążenie / Transaction category (credit/debit)
+      transactionStatus:
+        $ref: #/definitions/DictionaryItem
+      initiator:
+        $ref: #/definitions/NameAddress
+      sender:
+        $ref: #/definitions/SenderRecipient
+      recipient:
+        $ref: #/definitions/SenderRecipient
 • xml:
   name: TransactionCancelledInfo</t>
         </is>
@@ -6988,27 +6988,27 @@
           <t>Removed:
 • description: Klasa opisująca zaplanowaną transakcję płatniczą
 • allOf:
-  $ref: #/definitions/ItemInfoBase
-  type: object
-  required:
-    - itemId
-    - amount
-    - transactionCategory
-  properties:
-    transactionCategory:
-      type: string
-      enum:
-        - CREDIT
-        - DEBIT
-      description: Kategoria transakcji uznanie/obciążenie / Transaction category (credit/debit)
-    transactionStatus:
-      $ref: #/definitions/DictionaryItem
-    initiator:
-      $ref: #/definitions/NameAddress
-    sender:
-      $ref: #/definitions/SenderRecipient
-    recipient:
-      $ref: #/definitions/SenderRecipient
+  -     $ref: #/definitions/ItemInfoBase
+  -     type: object
+    required:
+      -         itemId
+      -         amount
+      -         transactionCategory
+    properties:
+      transactionCategory:
+        type: string
+        enum:
+          -             CREDIT
+          -             DEBIT
+        description: Kategoria transakcji uznanie/obciążenie / Transaction category (credit/debit)
+      transactionStatus:
+        $ref: #/definitions/DictionaryItem
+      initiator:
+        $ref: #/definitions/NameAddress
+      sender:
+        $ref: #/definitions/SenderRecipient
+      recipient:
+        $ref: #/definitions/SenderRecipient
 • xml:
   name: TransactionScheduledInfo</t>
         </is>
@@ -7051,7 +7051,7 @@
           <t>Removed:
 • description: Klasa odpowiedzi zawierająca listę transakcji done / Done Transaction Information Response Class
 • required:
-  - responseHeader
+  -     responseHeader
 • properties:
   responseHeader:
     $ref: #/definitions/ResponseHeader
@@ -7103,7 +7103,7 @@
           <t>Removed:
 • description: Klasa odpowiedzi zawierająca listę transakcji cancelled / Cancelled Transaction Information Response Class
 • required:
-  - responseHeader
+  -     responseHeader
 • properties:
   responseHeader:
     $ref: #/definitions/ResponseHeader
@@ -7155,7 +7155,7 @@
           <t>Removed:
 • description: Klasa odpowiedzi zawierająca listę transakcji scheduled / Scheduled Transaction Information Response Class
 • required:
-  - responseHeader
+  -     responseHeader
 • properties:
   responseHeader:
     $ref: #/definitions/ResponseHeader
@@ -7207,7 +7207,7 @@
           <t>Removed:
 • description: Klasa odpowiedzi zawierająca listę transakcji pending / Pending Transaction Information Response Class
 • required:
-  - responseHeader
+  -     responseHeader
 • properties:
   responseHeader:
     $ref: #/definitions/ResponseHeader
@@ -7259,7 +7259,7 @@
           <t>Removed:
 • description: Klasa odpowiedzi zawierająca listę transakcji rejected / Rejected Transaction Information Response Class
 • required:
-  - responseHeader
+  -     responseHeader
 • properties:
   responseHeader:
     $ref: #/definitions/ResponseHeader
@@ -7311,7 +7311,7 @@
           <t>Removed:
 • description: Klasa odpowiedzi zawierająca listę blokad na rachunku / Hold Information Response Class
 • required:
-  - responseHeader
+  -     responseHeader
 • properties:
   responseHeader:
     $ref: #/definitions/ResponseHeader
@@ -7375,9 +7375,9 @@
 • description: Klasa zapytania o pojedynczą transakcję / Transaction Detail Request Class
 • type: object
 • required:
-  - requestHeader
-  - itemId
-  - accountNumber
+  -     requestHeader
+  -     itemId
+  -     accountNumber
 • properties:
   requestHeader:
     $ref: #/definitions/RequestHeaderAIS
@@ -7425,7 +7425,7 @@
       <c r="E117" s="7" t="inlineStr">
         <is>
           <t>Added:
-Typ identyfikatora płatnika / Payor ID type
+• Typ identyfikatora płatnika / Payor ID type
 * `N` - NIP
 * `P` - Pesel
 * `R` - Regon
@@ -7471,17 +7471,17 @@
       <c r="E118" s="7" t="inlineStr">
         <is>
           <t>Added:
-1
+• 1
 Added:
-2
+• 2
 Added:
-3
+• 3
 Removed:
-1
+• 1
 Removed:
-2
+• 2
 Removed:
-3</t>
+• 3</t>
         </is>
       </c>
     </row>
@@ -7521,18 +7521,18 @@
           <t>Removed:
 • name: payorIdType
 • values:
-  value: N
-  description: NIP
-  value: P
-  description: Pesel
-  value: R
-  description: Regon
-  value: 1
-  description: Dowód osobisty
-  value: 2
-  description: Paszport
-  value: 3
-  description: Inny</t>
+  -     value: N
+    description: NIP
+  -     value: P
+    description: Pesel
+  -     value: R
+    description: Regon
+  -     value: 1
+    description: Dowód osobisty
+  -     value: 2
+    description: Paszport
+  -     value: 3
+    description: Inny</t>
         </is>
       </c>
     </row>
@@ -7606,21 +7606,21 @@
     type: string
     description: Typ dodatkowego identyfikatora płatnika / Payor's additional identifier type
     enum:
-      - P
-      - R
-      - 1
-      - 2
+      -         P
+      -         R
+      -         1
+      -         2
     x-ms-enum:
       name: additionalPayorIdType
       values:
-        value: P
-        description: Pesel
-        value: R
-        description: Regon
-        value: 1
-        description: Dowód osobisty
-        value: 2
-        description: Paszport
+        -           value: P
+          description: Pesel
+        -           value: R
+          description: Regon
+        -           value: 1
+          description: Dowód osobisty
+        -           value: 2
+          description: Paszport
 • xml:
   name: SocialSecurityPayor</t>
         </is>
@@ -7829,8 +7829,8 @@
 • description: Klasa odpowiedzi na zapytanie o transakcję /  Transaction Detail Response Class
 • type: object
 • required:
-  - responseHeader
-  - baseInfo
+  -     responseHeader
+  -     baseInfo
 • properties:
   responseHeader:
     $ref: #/definitions/ResponseHeader
@@ -7914,11 +7914,11 @@
       <c r="E124" s="7" t="inlineStr">
         <is>
           <t>Removed:
-ExpressElixir
+• ExpressElixir
 Removed:
-Sorbnet
+• Sorbnet
 Removed:
-BlueCash</t>
+• BlueCash</t>
         </is>
       </c>
     </row>
@@ -7951,7 +7951,7 @@
       <c r="E125" s="7" t="inlineStr">
         <is>
           <t>Added:
-UrgentD1</t>
+• UrgentD1</t>
         </is>
       </c>
     </row>
@@ -7987,9 +7987,9 @@
       <c r="E126" s="7" t="inlineStr">
         <is>
           <t>Added:
-Swift
+• Swift
 Added:
-SantanderOnePayFX</t>
+• SantanderOnePayFX</t>
         </is>
       </c>
     </row>
@@ -8019,7 +8019,7 @@
       <c r="E127" s="7" t="inlineStr">
         <is>
           <t>Added:
-#/definitions/PaymentNonEEARequestBank</t>
+• #/definitions/PaymentNonEEARequestBank</t>
         </is>
       </c>
     </row>
@@ -8052,11 +8052,11 @@
       <c r="E128" s="7" t="inlineStr">
         <is>
           <t>Added:
-SEPA
+• SEPA
 Added:
-Target
+• Target
 Added:
-SantanderOnePayFX</t>
+• SantanderOnePayFX</t>
         </is>
       </c>
     </row>
@@ -8082,7 +8082,7 @@
       <c r="E129" s="7" t="inlineStr">
         <is>
           <t>Added:
-object</t>
+• object</t>
         </is>
       </c>
     </row>
@@ -8108,7 +8108,7 @@
       <c r="E130" s="7" t="inlineStr">
         <is>
           <t>Added:
-object</t>
+• object</t>
         </is>
       </c>
     </row>
@@ -8134,7 +8134,7 @@
       <c r="E131" s="7" t="inlineStr">
         <is>
           <t>Added:
-object</t>
+• object</t>
         </is>
       </c>
     </row>
@@ -8160,7 +8160,7 @@
       <c r="E132" s="7" t="inlineStr">
         <is>
           <t>Added:
-35</t>
+• 35</t>
         </is>
       </c>
     </row>
@@ -8193,11 +8193,11 @@
       <c r="E133" s="7" t="inlineStr">
         <is>
           <t>Removed:
-EEA
+• EEA
 Removed:
-nonEEA
+• nonEEA
 Removed:
-tax</t>
+• tax</t>
         </is>
       </c>
     </row>
@@ -8298,7 +8298,7 @@
       <c r="E137" s="7" t="inlineStr">
         <is>
           <t>Added:
-object</t>
+• object</t>
         </is>
       </c>
     </row>
@@ -8324,7 +8324,7 @@
       <c r="E138" s="7" t="inlineStr">
         <is>
           <t>Added:
-object</t>
+• object</t>
         </is>
       </c>
     </row>
@@ -8350,7 +8350,7 @@
       <c r="E139" s="7" t="inlineStr">
         <is>
           <t>Added:
-object</t>
+• object</t>
         </is>
       </c>
     </row>
@@ -8376,7 +8376,7 @@
       <c r="E140" s="7" t="inlineStr">
         <is>
           <t>Added:
-object</t>
+• object</t>
         </is>
       </c>
     </row>
@@ -8402,7 +8402,7 @@
       <c r="E141" s="7" t="inlineStr">
         <is>
           <t>Added:
-object</t>
+• object</t>
         </is>
       </c>
     </row>
@@ -8428,7 +8428,7 @@
       <c r="E142" s="7" t="inlineStr">
         <is>
           <t>Added:
-object</t>
+• object</t>
         </is>
       </c>
     </row>
@@ -8454,7 +8454,7 @@
       <c r="E143" s="7" t="inlineStr">
         <is>
           <t>Added:
-object</t>
+• object</t>
         </is>
       </c>
     </row>
@@ -8480,7 +8480,7 @@
       <c r="E144" s="7" t="inlineStr">
         <is>
           <t>Added:
-object</t>
+• object</t>
         </is>
       </c>
     </row>
@@ -8506,7 +8506,7 @@
       <c r="E145" s="7" t="inlineStr">
         <is>
           <t>Added:
-object</t>
+• object</t>
         </is>
       </c>
     </row>
@@ -8532,7 +8532,7 @@
       <c r="E146" s="7" t="inlineStr">
         <is>
           <t>Added:
-object</t>
+• object</t>
         </is>
       </c>
     </row>
@@ -8557,7 +8557,7 @@
       <c r="E147" s="7" t="inlineStr">
         <is>
           <t>Removed:
-Klasa odpowiedzi na pytanie o płatność / Payment Get Response Class</t>
+• Klasa odpowiedzi na pytanie o płatność / Payment Get Response Class</t>
         </is>
       </c>
     </row>
@@ -8606,15 +8606,15 @@
   responseHeader:
     $ref: #/definitions/ResponseHeader
 • required:
-  - responseHeader
+  -     responseHeader
 • type: object
 Removed:
 • type: object
 • required:
-  - responseHeader
-  - paymentId
-  - generalStatus
-  - detailedStatus
+  -     responseHeader
+  -     paymentId
+  -     generalStatus
+  -     detailedStatus
 • properties:
   responseHeader:
     $ref: #/definitions/ResponseHeader</t>
@@ -8643,7 +8643,7 @@
       <c r="E149" s="7" t="inlineStr">
         <is>
           <t>Added:
-object</t>
+• object</t>
         </is>
       </c>
     </row>
@@ -8669,7 +8669,7 @@
       <c r="E150" s="7" t="inlineStr">
         <is>
           <t>Added:
-object</t>
+• object</t>
         </is>
       </c>
     </row>
@@ -8695,7 +8695,7 @@
       <c r="E151" s="7" t="inlineStr">
         <is>
           <t>Added:
-object</t>
+• object</t>
         </is>
       </c>
     </row>
@@ -8748,10 +8748,10 @@
 • description: Klasa zapytania o dostępne środki płatnicze na rachunku / Confirmation of Funds Request Class
 • type: object
 • required:
-  - requestHeader
-  - accountNumber
-  - amount
-  - currency
+  -     requestHeader
+  -     accountNumber
+  -     amount
+  -     currency
 • properties:
   requestHeader:
     $ref: #/definitions/RequestHeaderWithoutToken
@@ -8809,8 +8809,8 @@
           <t>Removed:
 • description: Klasa odpowiedzi na zapytanie o dostępne środki płatnicze na rachunku / Confirmation of Funds Response Class
 • required:
-  - responseHeader
-  - fundsAvailable
+  -     responseHeader
+  -     fundsAvailable
 • properties:
   responseHeader:
     $ref: #/definitions/ResponseHeader
@@ -8818,8 +8818,8 @@
     description: Status - Czy środki są dostępne / Status - are funds available
     type: boolean
     enum:
-      - True
-      - False</t>
+      -         True
+      -         False</t>
         </is>
       </c>
     </row>
@@ -8845,7 +8845,7 @@
       <c r="E154" s="7" t="inlineStr">
         <is>
           <t>Added:
-object</t>
+• object</t>
         </is>
       </c>
     </row>
@@ -8871,7 +8871,7 @@
       <c r="E155" s="7" t="inlineStr">
         <is>
           <t>Added:
-255</t>
+• 255</t>
         </is>
       </c>
     </row>
@@ -8897,7 +8897,7 @@
       <c r="E156" s="7" t="inlineStr">
         <is>
           <t>Added:
-255</t>
+• 255</t>
         </is>
       </c>
     </row>
@@ -8923,7 +8923,7 @@
       <c r="E157" s="7" t="inlineStr">
         <is>
           <t>Added:
-127</t>
+• 127</t>
         </is>
       </c>
     </row>
@@ -8989,24 +8989,24 @@
           <t>Removed:
 • description: Klasa zawierająca informacje o PSU na potrzeby usług autoryzacji / PSU Information Class dedicated for authorization services
 • allOf:
-  $ref: #/definitions/RequestHeaderWithoutToken
-  type: object
-  properties:
-    isCompanyContext:
-      type: boolean
-      description: (true / false) Znacznik oznaczający czy żądanie jest wysyłane w kontekście PSU korporacyjnego
-    psuIdentifierType:
-      type: string
-      description: Typ identyfikatora PSU, służy do wskazania przez TPP na podstawie jakiej informacji zostanie zidentyfikowany PSU, który będzie podlegał uwierzytelnieniu. Wartość słownikowa. / PSU identifier type, used by TPP to indicate type of information based on which the PSU is to be authenticated. Dictionary value.
-    psuIdentifierValue:
-      type: string
-      description: Wartość identyfikatora PSU. Wymagany warunkowo - w przypadku gdy została przekazana niepusta wartość typu identyfikatora PSU. / The value of the PSU's identifier. Required conditionally - in case non empty value of PSU identifier type was passed.
-    psuContextIdentifierType:
-      type: string
-      description: Typ identyfikatora kontekstu w jakim występuje PSU. Wartość słownikowa. Wymagany warunkowo - w przypadku wysyłania żądania dla takiego PSU, który może występować w więcej niż jednym kontekście w wybranym ASPSP. / Identifier of context that is used by PSU. Dictionary value. Required conditionally - in case context of the request is used and PSU may use more then one context for the ASPSP.
-    psuContextIdentifierValue:
-      type: string
-      description: Wartość identyfikatora kontekstu w jakim występuje PSU. Wymagany warunkowo - w przypadku wysyłania żądania dla takiego PSU, który może występować w więcej niż jednym kontekście w wybranym ASPSP. / The value of context that is used by PSU. Required conditionally - in case context of the request is used and PSU may use more then one context for the ASPSP.</t>
+  -     $ref: #/definitions/RequestHeaderWithoutToken
+  -     type: object
+    properties:
+      isCompanyContext:
+        type: boolean
+        description: (true / false) Znacznik oznaczający czy żądanie jest wysyłane w kontekście PSU korporacyjnego
+      psuIdentifierType:
+        type: string
+        description: Typ identyfikatora PSU, służy do wskazania przez TPP na podstawie jakiej informacji zostanie zidentyfikowany PSU, który będzie podlegał uwierzytelnieniu. Wartość słownikowa. / PSU identifier type, used by TPP to indicate type of information based on which the PSU is to be authenticated. Dictionary value.
+      psuIdentifierValue:
+        type: string
+        description: Wartość identyfikatora PSU. Wymagany warunkowo - w przypadku gdy została przekazana niepusta wartość typu identyfikatora PSU. / The value of the PSU's identifier. Required conditionally - in case non empty value of PSU identifier type was passed.
+      psuContextIdentifierType:
+        type: string
+        description: Typ identyfikatora kontekstu w jakim występuje PSU. Wartość słownikowa. Wymagany warunkowo - w przypadku wysyłania żądania dla takiego PSU, który może występować w więcej niż jednym kontekście w wybranym ASPSP. / Identifier of context that is used by PSU. Dictionary value. Required conditionally - in case context of the request is used and PSU may use more then one context for the ASPSP.
+      psuContextIdentifierValue:
+        type: string
+        description: Wartość identyfikatora kontekstu w jakim występuje PSU. Wymagany warunkowo - w przypadku wysyłania żądania dla takiego PSU, który może występować w więcej niż jednym kontekście w wybranym ASPSP. / The value of context that is used by PSU. Required conditionally - in case context of the request is used and PSU may use more then one context for the ASPSP.</t>
         </is>
       </c>
     </row>
@@ -9046,17 +9046,17 @@
           <t>Removed:
 • description: Klasa zawierająca informacje o PSU and callback URL / PSU and callback URL Information Class
 • allOf:
-  $ref: #/definitions/RequestHeaderWithoutTokenAS
-  type: object
-  required:
-    - callbackURL, apiKey
-  properties:
-    callbackURL:
-      type: string
-      description: adres funkcji zwrotnej / callback URL
-    apiKey:
-      type: string
-      description: API key dla wywołania funkcji zwrotnej / callback API key</t>
+  -     $ref: #/definitions/RequestHeaderWithoutTokenAS
+  -     type: object
+    required:
+      -         callbackURL, apiKey
+    properties:
+      callbackURL:
+        type: string
+        description: adres funkcji zwrotnej / callback URL
+      apiKey:
+        type: string
+        description: API key dla wywołania funkcji zwrotnej / callback API key</t>
         </is>
       </c>
     </row>
@@ -9082,7 +9082,7 @@
       <c r="E160" s="7" t="inlineStr">
         <is>
           <t>Removed:
-Klasa zawierająca informacje o PSU and callback URL / PSU and callback URL Information Class</t>
+• Klasa zawierająca informacje o PSU and callback URL / PSU and callback URL Information Class</t>
         </is>
       </c>
     </row>
@@ -9155,12 +9155,12 @@
     maxLength: 255
     type: string
 • required:
-  - token
+  -     token
 • type: object
 Removed:
 • type: object
 • required:
-  - token
+  -     token
 • properties:
   token:
     type: string
@@ -9195,7 +9195,7 @@
       <c r="E162" s="7" t="inlineStr">
         <is>
           <t>Removed:
-Klasa zawierająca informacje o PSU / PSU Information Class</t>
+• Klasa zawierająca informacje o PSU / PSU Information Class</t>
         </is>
       </c>
     </row>
@@ -9246,12 +9246,12 @@
     maxLength: 256
     type: string
 • required:
-  - token
+  -     token
 • type: object
 Removed:
 • type: object
 • required:
-  - token
+  -     token
 • properties:
   token:
     type: string
@@ -9296,17 +9296,17 @@
           <t>Removed:
 • description: Klasa zawierająca informacje o PSU / PSU Information Class
 • allOf:
-  $ref: #/definitions/RequestHeaderWithoutToken
-  type: object
-  required:
-    - token
-  properties:
-    token:
-      type: string
-      description: Token autoryzacyjny / Authorization token
-    isDirectPsu:
-      type: boolean
-      description: (true/false) Znacznik informujący czy request jest przesłany bezpośrednio przez PSU. Domyślna wartość to false. / Is request sent by PSU directly. false is default value.</t>
+  -     $ref: #/definitions/RequestHeaderWithoutToken
+  -     type: object
+    required:
+      -         token
+    properties:
+      token:
+        type: string
+        description: Token autoryzacyjny / Authorization token
+      isDirectPsu:
+        type: boolean
+        description: (true/false) Znacznik informujący czy request jest przesłany bezpośrednio przez PSU. Domyślna wartość to false. / Is request sent by PSU directly. false is default value.</t>
         </is>
       </c>
     </row>
@@ -9354,23 +9354,23 @@
           <t>Removed:
 • description: Klasa zawierająca informacje o PSU and callback URL / PSU and callback URL Information Class
 • allOf:
-  $ref: #/definitions/RequestHeaderWithoutToken
-  type: object
-  required:
-    - token
-  properties:
-    token:
-      type: string
-      description: Token autoryzacyjny / Authorization token
-    isDirectPsu:
-      type: boolean
-      description: (true/false) Znacznik informujący czy request jest przesłany bezpośrednio przez PSU. Domyślna wartość to false. / Is request sent by PSU directly. false is default value.
-    callbackURL:
-      type: string
-      description: adres funkcji zwrotnej / callback URL
-    apiKey:
-      type: string
-      description: API key dla wywołania funkcji zwrotnej / callback API key</t>
+  -     $ref: #/definitions/RequestHeaderWithoutToken
+  -     type: object
+    required:
+      -         token
+    properties:
+      token:
+        type: string
+        description: Token autoryzacyjny / Authorization token
+      isDirectPsu:
+        type: boolean
+        description: (true/false) Znacznik informujący czy request jest przesłany bezpośrednio przez PSU. Domyślna wartość to false. / Is request sent by PSU directly. false is default value.
+      callbackURL:
+        type: string
+        description: adres funkcji zwrotnej / callback URL
+      apiKey:
+        type: string
+        description: API key dla wywołania funkcji zwrotnej / callback API key</t>
         </is>
       </c>
     </row>
@@ -9396,7 +9396,7 @@
       <c r="E166" s="7" t="inlineStr">
         <is>
           <t>Removed:
-uuid</t>
+• uuid</t>
         </is>
       </c>
     </row>
@@ -9422,7 +9422,7 @@
       <c r="E167" s="7" t="inlineStr">
         <is>
           <t>Added:
-object</t>
+• object</t>
         </is>
       </c>
     </row>
@@ -9448,7 +9448,7 @@
       <c r="E168" s="7" t="inlineStr">
         <is>
           <t>Added:
-object</t>
+• object</t>
         </is>
       </c>
     </row>
@@ -9474,7 +9474,7 @@
       <c r="E169" s="7" t="inlineStr">
         <is>
           <t>Added:
-object</t>
+• object</t>
         </is>
       </c>
     </row>
@@ -9500,7 +9500,7 @@
       <c r="E170" s="7" t="inlineStr">
         <is>
           <t>Added:
-object</t>
+• object</t>
         </is>
       </c>
     </row>
@@ -9578,7 +9578,7 @@
       <c r="E172" s="7" t="inlineStr">
         <is>
           <t>Removed:
-before</t>
+• before</t>
         </is>
       </c>
     </row>
@@ -9662,7 +9662,7 @@
       <c r="E174" s="7" t="inlineStr">
         <is>
           <t>Added:
-35</t>
+• 35</t>
         </is>
       </c>
     </row>
@@ -9688,7 +9688,7 @@
       <c r="E175" s="7" t="inlineStr">
         <is>
           <t>Removed:
-10</t>
+• 10</t>
         </is>
       </c>
     </row>
@@ -9719,7 +9719,7 @@
       <c r="E176" s="7" t="inlineStr">
         <is>
           <t>Added:
-Bazowa klasa dla TransferData / TransferData Base Class</t>
+• Bazowa klasa dla TransferData / TransferData Base Class</t>
         </is>
       </c>
     </row>
@@ -9753,16 +9753,16 @@
       <c r="E177" s="7" t="inlineStr">
         <is>
           <t>Removed:
-$ref: #/definitions/TransferDataBase
-type: object
-required:
-  - description
-  - amount
-properties:
-  currency:
-    type: string
-    maxLength: 3
-    description: Waluta / Currency</t>
+•   $ref: #/definitions/TransferDataBase
+•   type: object
+  required:
+    -       description
+    -       amount
+  properties:
+    currency:
+      type: string
+      maxLength: 3
+      description: Waluta / Currency</t>
         </is>
       </c>
     </row>
@@ -9848,8 +9848,8 @@
       <c r="E179" s="7" t="inlineStr">
         <is>
           <t>Added:
-• amount
-• description</t>
+•   amount
+•   description</t>
         </is>
       </c>
     </row>
@@ -9875,7 +9875,7 @@
       <c r="E180" s="7" t="inlineStr">
         <is>
           <t>Added:
-object</t>
+• object</t>
         </is>
       </c>
     </row>
@@ -9906,7 +9906,7 @@
       <c r="E181" s="7" t="inlineStr">
         <is>
           <t>Added:
-Bazowa klasa dla TransferData / TransferData Base Class</t>
+• Bazowa klasa dla TransferData / TransferData Base Class</t>
         </is>
       </c>
     </row>
@@ -9941,17 +9941,17 @@
       <c r="E182" s="7" t="inlineStr">
         <is>
           <t>Removed:
-$ref: #/definitions/TransferDataBase
-type: object
-required:
-  - description
-  - amount
-  - currency
-properties:
-  currency:
-    type: string
-    maxLength: 3
-    description: Waluta, domyślnie EUR przelewów zagranicznych / Currency</t>
+•   $ref: #/definitions/TransferDataBase
+•   type: object
+  required:
+    -       description
+    -       amount
+    -       currency
+  properties:
+    currency:
+      type: string
+      maxLength: 3
+      description: Waluta, domyślnie EUR przelewów zagranicznych / Currency</t>
         </is>
       </c>
     </row>
@@ -10038,9 +10038,9 @@
       <c r="E184" s="7" t="inlineStr">
         <is>
           <t>Added:
-• currency
-• amount
-• description</t>
+•   currency
+•   amount
+•   description</t>
         </is>
       </c>
     </row>
@@ -10066,7 +10066,7 @@
       <c r="E185" s="7" t="inlineStr">
         <is>
           <t>Added:
-object</t>
+• object</t>
         </is>
       </c>
     </row>
@@ -10091,7 +10091,7 @@
       <c r="E186" s="7" t="inlineStr">
         <is>
           <t>Removed:
-Klasa zawierająca dane przelewu / Transfer Data Class</t>
+• Klasa zawierająca dane przelewu / Transfer Data Class</t>
         </is>
       </c>
     </row>
@@ -10126,16 +10126,16 @@
       <c r="E187" s="7" t="inlineStr">
         <is>
           <t>Removed:
-$ref: #/definitions/TransferDataBaseTax
-type: object
-required:
-  - amount
-  - currency
-properties:
-  currency:
-    type: string
-    maxLength: 3
-    description: Waluta, wymagana wartość PLN / Currency - PLN value required</t>
+•   $ref: #/definitions/TransferDataBaseTax
+•   type: object
+  required:
+    -       amount
+    -       currency
+  properties:
+    currency:
+      type: string
+      maxLength: 3
+      description: Waluta, wymagana wartość PLN / Currency - PLN value required</t>
         </is>
       </c>
     </row>
@@ -10213,8 +10213,8 @@
       <c r="E189" s="7" t="inlineStr">
         <is>
           <t>Added:
-• currency
-• amount</t>
+•   currency
+•   amount</t>
         </is>
       </c>
     </row>
@@ -10240,7 +10240,7 @@
       <c r="E190" s="7" t="inlineStr">
         <is>
           <t>Added:
-object</t>
+• object</t>
         </is>
       </c>
     </row>
@@ -10341,7 +10341,7 @@
       <c r="E193" s="7" t="inlineStr">
         <is>
           <t>Added:
-object</t>
+• object</t>
         </is>
       </c>
     </row>
@@ -10394,7 +10394,7 @@
       <c r="E195" s="7" t="inlineStr">
         <is>
           <t>Added:
-object</t>
+• object</t>
         </is>
       </c>
     </row>
@@ -10447,7 +10447,7 @@
       <c r="E197" s="7" t="inlineStr">
         <is>
           <t>Added:
-object</t>
+• object</t>
         </is>
       </c>
     </row>
@@ -10472,7 +10472,7 @@
       <c r="E198" s="7" t="inlineStr">
         <is>
           <t>Added:
-• value</t>
+•   value</t>
         </is>
       </c>
     </row>
@@ -10498,7 +10498,7 @@
       <c r="E199" s="7" t="inlineStr">
         <is>
           <t>Added:
-object</t>
+• object</t>
         </is>
       </c>
     </row>
@@ -10728,10 +10728,10 @@
 • description: Zakres, limity, parametry i czas ważności zgód, o które prosi TPP. / Scope, limits, parameters and expiration time of consents requested by TPP
 • type: object
 • required:
-  - consentId
-  - scopeGroupType
-  - scopeTimeLimit
-  - throttlingPolicy
+  -     consentId
+  -     scopeGroupType
+  -     scopeTimeLimit
+  -     throttlingPolicy
 • properties:
   privilegeList:
     type: array
@@ -10742,9 +10742,9 @@
     type: string
     description: Type of consent
     enum:
-      - ais-accounts
-      - ais
-      - pis
+      -         ais-accounts
+      -         ais
+      -         pis
   consentId:
     type: string
     description: Id of consent
@@ -10756,7 +10756,7 @@
     type: string
     description: Throttling policy
     enum:
-      - psd2Regulatory</t>
+      -         psd2Regulatory</t>
         </is>
       </c>
     </row>
@@ -10851,9 +10851,9 @@
 • description: Zakres, limity, parametry i czas ważności zgód, które potwierdza ASPSP / Scope, limits, parameters and expiration time of consents that are confimed by ASPSP
 • type: object
 • required:
-  - consentId
-  - scopeTimeLimit
-  - throttlingPolicy
+  -     consentId
+  -     scopeTimeLimit
+  -     throttlingPolicy
 • properties:
   privilegeList:
     type: array
@@ -10871,13 +10871,13 @@
     type: string
     description: Throttling policy
     enum:
-      - psd2Regulatory
+      -         psd2Regulatory
 • example:
   consentId: consentId
   resource:
     accounts:
-      - accounts
-      - accounts
+      -         accounts
+      -         accounts
   scopeTimeLimit: scopeTimeLimit
   throttlingPolicy: psd2Regulatory
   privilegeList:
@@ -10953,8 +10953,8 @@
   scopeUsageLimit:
     type: string
     enum:
-      - single
-      - multiple
+      -         single
+      -         multiple
     description: Rodzaj limitu zgody / Type of limit of usages</t>
         </is>
       </c>
@@ -11004,13 +11004,13 @@
 • description: Lista atrybutów uprawnienia usługi AIS będących przedmiotem zapytania o zgodę PSU / The list of attributes of the privilege of the AIS service that are the subject of the request for PSU's consent
 • type: object
 • required:
-  - maxAllowedHistoryLong
+  -     maxAllowedHistoryLong
 • properties:
   scopeUsageLimit:
     type: string
     enum:
-      - single
-      - multiple
+      -         single
+      -         multiple
     description: Rodzaj limitu zgody / Type of limit of usages
   maxAllowedHistoryLong:
     type: integer
@@ -11057,8 +11057,8 @@
   scopeUsageLimit:
     type: string
     enum:
-      - single
-      - multiple
+      -         single
+      -         multiple
     description: Rodzaj limitu zgody / Type of limit of usages</t>
         </is>
       </c>
@@ -11111,13 +11111,13 @@
 • description: Lista atrybutów uprawnienia usługi AIS dla których została wyrażona zgoda przez PSU / The list of attributes of the privilege of the AIS service that the PSU's consent has been confirmed
 • type: object
 • required:
-  - maxAllowedHistoryLong
+  -     maxAllowedHistoryLong
 • properties:
   scopeUsageLimit:
     type: string
     enum:
-      - single
-      - multiple
+      -         single
+      -         multiple
     description: Rodzaj limitu zgody / Type of limit of usages
   maxAllowedHistoryLong:
     type: integer
@@ -11173,8 +11173,8 @@
   scopeUsageLimit:
     type: string
     enum:
-      - single
-      - multiple
+      -         single
+      -         multiple
     description: Rodzaj limitu zgody / Type of limit of usages
   paymentId:
     type: string
@@ -11228,8 +11228,8 @@
   scopeUsageLimit:
     type: string
     enum:
-      - single
-      - multiple
+      -         single
+      -         multiple
     description: Rodzaj limitu zgody / Type of limit of usages
   bundleId:
     type: string
@@ -11285,8 +11285,8 @@
   scopeUsageLimit:
     type: string
     enum:
-      - single
-      - multiple
+      -         single
+      -         multiple
     description: Rodzaj limitu zgody / Type of limit of usages
   recurringPaymentId:
     type: string
@@ -11364,8 +11364,8 @@
   scopeUsageLimit:
     type: string
     enum:
-      - single
-      - multiple
+      -         single
+      -         multiple
     description: Rodzaj limitu zgody / Type of limit of usages
   recipient:
     $ref: #/definitions/RecipientPIS
@@ -11377,23 +11377,23 @@
     description: Tryb pilności / Urgency mode
     type: string
     enum:
-      - ExpressD0
-      - StandardD1
+      -         ExpressD0
+      -         StandardD1
   system:
     description: Droga jaką przelew ma być rozliczony / The way the transfer should be settled
     type: string
     enum:
-      - Elixir
-      - ExpressElixir
-      - Sorbnet
-      - BlueCash
-      - Internal
+      -         Elixir
+      -         ExpressElixir
+      -         Sorbnet
+      -         BlueCash
+      -         Internal
   executionMode:
     description: Tryb realizacji płatności. Nadrzędna informacja decydująca o tym w jakim trybie zostanie zrealizowana płatność. / Payment execution mode. The superior information deciding which mode is to be used to execute payment.
     type: string
     enum:
-      - Immediate
-      - FutureDated</t>
+      -         Immediate
+      -         FutureDated</t>
         </is>
       </c>
     </row>
@@ -11462,8 +11462,8 @@
   scopeUsageLimit:
     type: string
     enum:
-      - single
-      - multiple
+      -         single
+      -         multiple
     description: Rodzaj limitu zgody / Type of limit of usages
   recipient:
     $ref: #/definitions/RecipientPISForeign
@@ -11475,21 +11475,21 @@
     description: Tryb pilności / Urgency mode
     type: string
     enum:
-      - ExpressD0
-      - StandardD1
+      -         ExpressD0
+      -         StandardD1
   system:
     description: Droga jaką przelew ma być rozliczony / The way the transfer should be settled
     type: string
     enum:
-      - SEPA
-      - InstantSEPA
-      - Target
+      -         SEPA
+      -         InstantSEPA
+      -         Target
   executionMode:
     description: Tryb realizacji płatności. Nadrzędna informacja decydująca o tym w jakim trybie zostanie zrealizowana płatność. / Payment execution mode. The superior information deciding which mode is to be used to execute payment.
     type: string
     enum:
-      - Immediate
-      - FutureDated</t>
+      -         Immediate
+      -         FutureDated</t>
         </is>
       </c>
     </row>
@@ -11564,8 +11564,8 @@
   scopeUsageLimit:
     type: string
     enum:
-      - single
-      - multiple
+      -         single
+      -         multiple
     description: Rodzaj limitu zgody / Type of limit of usages
   recipient:
     $ref: #/definitions/RecipientPISForeign
@@ -11583,20 +11583,20 @@
     description: Tryb pilności / Urgency mode
     type: string
     enum:
-      - ExpressD0
-      - UrgentD1
-      - StandardD2
+      -         ExpressD0
+      -         UrgentD1
+      -         StandardD2
   system:
     description: Droga jaką przelew ma być rozliczony / The way the transfer should be settled
     type: string
     enum:
-      - Swift
+      -         Swift
   executionMode:
     description: Tryb realizacji płatności. Nadrzędna informacja decydująca o tym w jakim trybie zostanie zrealizowana płatność. / Payment execution mode. The superior information deciding which mode is to be used to execute payment.
     type: string
     enum:
-      - Immediate
-      - FutureDated</t>
+      -         Immediate
+      -         FutureDated</t>
         </is>
       </c>
     </row>
@@ -11666,8 +11666,8 @@
   scopeUsageLimit:
     type: string
     enum:
-      - single
-      - multiple
+      -         single
+      -         multiple
     description: Rodzaj limitu zgody / Type of limit of usages
   recipient:
     $ref: #/definitions/RecipientPISTax
@@ -11681,20 +11681,20 @@
     description: Tryb pilności / Urgency mode
     type: string
     enum:
-      - ExpressD0
-      - StandardD1
+      -         ExpressD0
+      -         StandardD1
   system:
     description: Droga jaką przelew ma być rozliczony / The way the transfer should be settled
     type: string
     enum:
-      - Elixir
-      - ExpressElixir
+      -         Elixir
+      -         ExpressElixir
   executionMode:
     description: Tryb realizacji płatności. Nadrzędna informacja decydująca o tym w jakim trybie zostanie zrealizowana płatność. / Payment execution mode. The superior information deciding which mode is to be used to execute payment.
     type: string
     enum:
-      - Immediate
-      - FutureDated</t>
+      -         Immediate
+      -         FutureDated</t>
         </is>
       </c>
     </row>
@@ -11741,8 +11741,8 @@
   scopeUsageLimit:
     type: string
     enum:
-      - single
-      - multiple
+      -         single
+      -         multiple
     description: Rodzaj limitu zgody / Type of limit of usages
   paymentId:
     type: string
@@ -11795,8 +11795,8 @@
   scopeUsageLimit:
     type: string
     enum:
-      - single
-      - multiple
+      -         single
+      -         multiple
     description: Rodzaj limitu zgody / Type of limit of usages
   recurringPaymentId:
     type: string
@@ -11886,8 +11886,8 @@
   scopeUsageLimit:
     type: string
     enum:
-      - single
-      - multiple
+      -         single
+      -         multiple
     description: Rodzaj limitu zgody / Type of limit of usages
   transfersTotalAmount:
     description: Łączna kwota wszystkich przelewów z paczki / The total amount of all transfers from bundle
@@ -11897,10 +11897,10 @@
     description: Typ przelewów, które zostaną zlecone w ramach paczki / The type of transfers that will be initiated through the bundle
     type: string
     enum:
-      - domestic
-      - EEA
-      - nonEEA
-      - tax
+      -         domestic
+      -         EEA
+      -         nonEEA
+      -         tax
   domesticTransfers:
     description: Lista struktur danych przelewów zwykłych, które zostaną zlecone. Wymagane gdy typeOfTransfers = domestic. / The list of data structures of domestic transfers to be initiated. Required when typeOfTransfers = domestic.
     type: array
@@ -11981,8 +11981,8 @@
   scopeUsageLimit:
     type: string
     enum:
-      - single
-      - multiple
+      -         single
+      -         multiple
     description: Rodzaj limitu zgody / Type of limit of usages
   recurrence:
     $ref: #/definitions/RecurringTransferParameters
@@ -11990,10 +11990,10 @@
     description: Typ przelewu, który zostanie wykorzystany do zdefiniowania nowej płatności cyklicznej  / The type of payment that is to be used to define new recurring payment
     type: string
     enum:
-      - domestic
-      - EEA
-      - nonEEA
-      - tax
+      -         domestic
+      -         EEA
+      -         nonEEA
+      -         tax
   domesticPayment:
     $ref: #/definitions/RecurringDomesticPayment
   EEAPayment:

</xml_diff>

<commit_message>
Refactor report_generator.py to improve change formatting
</commit_message>
<xml_diff>
--- a/reports/report.xlsx
+++ b/reports/report.xlsx
@@ -582,7 +582,7 @@
         </is>
       </c>
     </row>
-    <row r="3" ht="30" customHeight="1">
+    <row r="3" ht="15" customHeight="1">
       <c r="A3" s="6" t="inlineStr">
         <is>
           <t>PIS</t>
@@ -595,12 +595,7 @@
       </c>
       <c r="C3" s="7" t="inlineStr"/>
       <c r="D3" s="7" t="inlineStr"/>
-      <c r="E3" s="7" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Removed:
-• </t>
-        </is>
-      </c>
+      <c r="E3" s="7" t="inlineStr"/>
     </row>
     <row r="4" ht="210" customHeight="1">
       <c r="A4" s="6" t="inlineStr">
@@ -803,7 +798,7 @@
         </is>
       </c>
     </row>
-    <row r="10" ht="30" customHeight="1">
+    <row r="10" ht="15" customHeight="1">
       <c r="A10" s="6" t="inlineStr">
         <is>
           <t>PIS</t>
@@ -816,12 +811,7 @@
       </c>
       <c r="C10" s="7" t="inlineStr"/>
       <c r="D10" s="7" t="inlineStr"/>
-      <c r="E10" s="7" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Removed:
-• </t>
-        </is>
-      </c>
+      <c r="E10" s="7" t="inlineStr"/>
     </row>
     <row r="11" ht="210" customHeight="1">
       <c r="A11" s="6" t="inlineStr">
@@ -1225,7 +1215,7 @@
         </is>
       </c>
     </row>
-    <row r="23" ht="30" customHeight="1">
+    <row r="23" ht="15" customHeight="1">
       <c r="A23" s="6" t="inlineStr">
         <is>
           <t>PIS</t>
@@ -1238,12 +1228,7 @@
       </c>
       <c r="C23" s="7" t="inlineStr"/>
       <c r="D23" s="7" t="inlineStr"/>
-      <c r="E23" s="7" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Removed:
-• </t>
-        </is>
-      </c>
+      <c r="E23" s="7" t="inlineStr"/>
     </row>
     <row r="24" ht="210" customHeight="1">
       <c r="A24" s="6" t="inlineStr">
@@ -1446,7 +1431,7 @@
         </is>
       </c>
     </row>
-    <row r="30" ht="30" customHeight="1">
+    <row r="30" ht="15" customHeight="1">
       <c r="A30" s="6" t="inlineStr">
         <is>
           <t>PIS</t>
@@ -1459,12 +1444,7 @@
       </c>
       <c r="C30" s="7" t="inlineStr"/>
       <c r="D30" s="7" t="inlineStr"/>
-      <c r="E30" s="7" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Removed:
-• </t>
-        </is>
-      </c>
+      <c r="E30" s="7" t="inlineStr"/>
     </row>
     <row r="31" ht="210" customHeight="1">
       <c r="A31" s="6" t="inlineStr">
@@ -1667,7 +1647,7 @@
         </is>
       </c>
     </row>
-    <row r="37" ht="30" customHeight="1">
+    <row r="37" ht="15" customHeight="1">
       <c r="A37" s="6" t="inlineStr">
         <is>
           <t>PIS</t>
@@ -1680,12 +1660,7 @@
       </c>
       <c r="C37" s="7" t="inlineStr"/>
       <c r="D37" s="7" t="inlineStr"/>
-      <c r="E37" s="7" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Removed:
-• </t>
-        </is>
-      </c>
+      <c r="E37" s="7" t="inlineStr"/>
     </row>
     <row r="38" ht="210" customHeight="1">
       <c r="A38" s="6" t="inlineStr">
@@ -7398,7 +7373,7 @@
         </is>
       </c>
     </row>
-    <row r="117" ht="120" customHeight="1">
+    <row r="117" ht="45" customHeight="1">
       <c r="A117" s="11" t="inlineStr">
         <is>
           <t>Definitions</t>
@@ -7425,13 +7400,7 @@
       <c r="E117" s="7" t="inlineStr">
         <is>
           <t>Added:
-• Typ identyfikatora płatnika / Payor ID type
-* `N` - NIP
-* `P` - Pesel
-* `R` - Regon
-* `1` - Dowód osobisty
-* `2` - Paszport
-* `3` - Inny</t>
+• Typ identyfikatora płatnika / Payor ID type</t>
         </is>
       </c>
     </row>
@@ -8019,7 +7988,7 @@
       <c r="E127" s="7" t="inlineStr">
         <is>
           <t>Added:
-• #/definitions/PaymentNonEEARequestBank</t>
+• #/definitions/Bank</t>
         </is>
       </c>
     </row>
@@ -9719,7 +9688,7 @@
       <c r="E176" s="7" t="inlineStr">
         <is>
           <t>Added:
-• Bazowa klasa dla TransferData / TransferData Base Class</t>
+• Klasa zawierająca dane przelewu / Transfer Data Class</t>
         </is>
       </c>
     </row>
@@ -9906,7 +9875,7 @@
       <c r="E181" s="7" t="inlineStr">
         <is>
           <t>Added:
-• Bazowa klasa dla TransferData / TransferData Base Class</t>
+• Klasa zawierająca dane przelewu / Transfer Data Class</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
deleted upload polish api section, it is now loaded in the program
</commit_message>
<xml_diff>
--- a/reports/report.xlsx
+++ b/reports/report.xlsx
@@ -571,7 +571,7 @@
         </is>
       </c>
     </row>
-    <row r="2" ht="210" customHeight="1">
+    <row r="2" ht="45" customHeight="1">
       <c r="A2" s="7" t="inlineStr">
         <is>
           <t>PIS</t>
@@ -579,15 +579,46 @@
       </c>
       <c r="B2" s="8" t="inlineStr">
         <is>
-          <t>UNCATEGORIZED</t>
+          <t>HIGH</t>
         </is>
       </c>
       <c r="C2" s="8" t="inlineStr">
         <is>
+          <t>/v2_1_1.1/payments/v2_1_1.1/domestic.x-swagger-router-controller</t>
+        </is>
+      </c>
+      <c r="D2" s="8" t="inlineStr">
+        <is>
+          <t xml:space="preserve">pis
+...
+</t>
+        </is>
+      </c>
+      <c r="E2" s="8" t="inlineStr"/>
+      <c r="F2" s="8" t="inlineStr">
+        <is>
+          <t>Removed:
+• pis</t>
+        </is>
+      </c>
+    </row>
+    <row r="3" ht="210" customHeight="1">
+      <c r="A3" s="7" t="inlineStr">
+        <is>
+          <t>PIS</t>
+        </is>
+      </c>
+      <c r="B3" s="8" t="inlineStr">
+        <is>
+          <t>UNCATEGORIZED</t>
+        </is>
+      </c>
+      <c r="C3" s="8" t="inlineStr">
+        <is>
           <t>/v2_1_1.1/payments/v2_1_1.1/domestic.post.parameters</t>
         </is>
       </c>
-      <c r="D2" s="8" t="inlineStr">
+      <c r="D3" s="8" t="inlineStr">
         <is>
           <t xml:space="preserve">- $ref: '#/parameters/authorizationParam'
 - $ref: '#/parameters/acceptEncodingParam'
@@ -604,7 +635,7 @@
 </t>
         </is>
       </c>
-      <c r="E2" s="8" t="inlineStr">
+      <c r="E3" s="8" t="inlineStr">
         <is>
           <t xml:space="preserve">- $ref: '#/parameters/authorizationParam'
 - $ref: '#/parameters/acceptEncodingParam'
@@ -622,30 +653,30 @@
 </t>
         </is>
       </c>
-      <c r="F2" s="8" t="inlineStr">
+      <c r="F3" s="8" t="inlineStr">
         <is>
           <t>Added:
 • $ref: #/parameters/contentTypeParam</t>
         </is>
       </c>
     </row>
-    <row r="3" ht="60" customHeight="1">
-      <c r="A3" s="7" t="inlineStr">
+    <row r="4" ht="60" customHeight="1">
+      <c r="A4" s="7" t="inlineStr">
         <is>
           <t>PIS</t>
         </is>
       </c>
-      <c r="B3" s="8" t="inlineStr">
-        <is>
-          <t>UNCATEGORIZED</t>
-        </is>
-      </c>
-      <c r="C3" s="8" t="inlineStr">
+      <c r="B4" s="8" t="inlineStr">
+        <is>
+          <t>UNCATEGORIZED</t>
+        </is>
+      </c>
+      <c r="C4" s="8" t="inlineStr">
         <is>
           <t>/v2_1_1.1/payments/v2_1_1.1/domestic.post.responses.500</t>
         </is>
       </c>
-      <c r="D3" s="8" t="inlineStr">
+      <c r="D4" s="8" t="inlineStr">
         <is>
           <t xml:space="preserve">description: Internal Server Error
 schema:
@@ -653,8 +684,8 @@
 </t>
         </is>
       </c>
-      <c r="E3" s="8" t="inlineStr"/>
-      <c r="F3" s="8" t="inlineStr">
+      <c r="E4" s="8" t="inlineStr"/>
+      <c r="F4" s="8" t="inlineStr">
         <is>
           <t>Removed:
 • description: Internal Server Error
@@ -663,23 +694,23 @@
         </is>
       </c>
     </row>
-    <row r="4" ht="60" customHeight="1">
-      <c r="A4" s="7" t="inlineStr">
+    <row r="5" ht="60" customHeight="1">
+      <c r="A5" s="7" t="inlineStr">
         <is>
           <t>PIS</t>
         </is>
       </c>
-      <c r="B4" s="8" t="inlineStr">
-        <is>
-          <t>UNCATEGORIZED</t>
-        </is>
-      </c>
-      <c r="C4" s="8" t="inlineStr">
+      <c r="B5" s="8" t="inlineStr">
+        <is>
+          <t>UNCATEGORIZED</t>
+        </is>
+      </c>
+      <c r="C5" s="8" t="inlineStr">
         <is>
           <t>/v2_1_1.1/payments/v2_1_1.1/domestic.post.responses.503</t>
         </is>
       </c>
-      <c r="D4" s="8" t="inlineStr">
+      <c r="D5" s="8" t="inlineStr">
         <is>
           <t xml:space="preserve">description: Service Unavailable
 schema:
@@ -687,8 +718,8 @@
 </t>
         </is>
       </c>
-      <c r="E4" s="8" t="inlineStr"/>
-      <c r="F4" s="8" t="inlineStr">
+      <c r="E5" s="8" t="inlineStr"/>
+      <c r="F5" s="8" t="inlineStr">
         <is>
           <t>Removed:
 • description: Service Unavailable
@@ -697,24 +728,24 @@
         </is>
       </c>
     </row>
-    <row r="5" ht="60" customHeight="1">
-      <c r="A5" s="7" t="inlineStr">
+    <row r="6" ht="60" customHeight="1">
+      <c r="A6" s="7" t="inlineStr">
         <is>
           <t>PIS</t>
         </is>
       </c>
-      <c r="B5" s="8" t="inlineStr">
-        <is>
-          <t>UNCATEGORIZED</t>
-        </is>
-      </c>
-      <c r="C5" s="8" t="inlineStr">
+      <c r="B6" s="8" t="inlineStr">
+        <is>
+          <t>UNCATEGORIZED</t>
+        </is>
+      </c>
+      <c r="C6" s="8" t="inlineStr">
         <is>
           <t>/v2_1_1.1/payments/v2_1_1.1/domestic.post.responses.510</t>
         </is>
       </c>
-      <c r="D5" s="8" t="inlineStr"/>
-      <c r="E5" s="8" t="inlineStr">
+      <c r="D6" s="8" t="inlineStr"/>
+      <c r="E6" s="8" t="inlineStr">
         <is>
           <t xml:space="preserve">description: Internal Server Error
 schema:
@@ -722,7 +753,7 @@
 </t>
         </is>
       </c>
-      <c r="F5" s="8" t="inlineStr">
+      <c r="F6" s="8" t="inlineStr">
         <is>
           <t>Added:
 • description: Internal Server Error
@@ -731,23 +762,23 @@
         </is>
       </c>
     </row>
-    <row r="6" ht="75" customHeight="1">
-      <c r="A6" s="7" t="inlineStr">
+    <row r="7" ht="75" customHeight="1">
+      <c r="A7" s="7" t="inlineStr">
         <is>
           <t>PIS</t>
         </is>
       </c>
-      <c r="B6" s="8" t="inlineStr">
-        <is>
-          <t>UNCATEGORIZED</t>
-        </is>
-      </c>
-      <c r="C6" s="8" t="inlineStr">
+      <c r="B7" s="8" t="inlineStr">
+        <is>
+          <t>UNCATEGORIZED</t>
+        </is>
+      </c>
+      <c r="C7" s="8" t="inlineStr">
         <is>
           <t>/v2_1_1.1/payments/v2_1_1.1/domestic.post.security</t>
         </is>
       </c>
-      <c r="D6" s="8" t="inlineStr">
+      <c r="D7" s="8" t="inlineStr">
         <is>
           <t xml:space="preserve">- xs2a_auth_aspsp:
   - pis
@@ -756,14 +787,14 @@
 </t>
         </is>
       </c>
-      <c r="E6" s="8" t="inlineStr">
+      <c r="E7" s="8" t="inlineStr">
         <is>
           <t xml:space="preserve">- xs2a_auth_decoupled:
   - pis
 </t>
         </is>
       </c>
-      <c r="F6" s="8" t="inlineStr">
+      <c r="F7" s="8" t="inlineStr">
         <is>
           <t>Removed:
 • xs2a_auth_aspsp:
@@ -771,54 +802,54 @@
         </is>
       </c>
     </row>
-    <row r="7" ht="45" customHeight="1">
-      <c r="A7" s="7" t="inlineStr">
+    <row r="8" ht="45" customHeight="1">
+      <c r="A8" s="7" t="inlineStr">
         <is>
           <t>PIS</t>
         </is>
       </c>
-      <c r="B7" s="8" t="inlineStr">
-        <is>
-          <t>UNCATEGORIZED</t>
-        </is>
-      </c>
-      <c r="C7" s="8" t="inlineStr">
+      <c r="B8" s="8" t="inlineStr">
+        <is>
+          <t>UNCATEGORIZED</t>
+        </is>
+      </c>
+      <c r="C8" s="8" t="inlineStr">
         <is>
           <t>/v2_1_1.1/payments/v2_1_1.1/EEA.x-swagger-router-controller</t>
         </is>
       </c>
-      <c r="D7" s="8" t="inlineStr">
+      <c r="D8" s="8" t="inlineStr">
         <is>
           <t xml:space="preserve">pis
 ...
 </t>
         </is>
       </c>
-      <c r="E7" s="8" t="inlineStr"/>
-      <c r="F7" s="8" t="inlineStr">
+      <c r="E8" s="8" t="inlineStr"/>
+      <c r="F8" s="8" t="inlineStr">
         <is>
           <t>Removed:
 • pis</t>
         </is>
       </c>
     </row>
-    <row r="8" ht="210" customHeight="1">
-      <c r="A8" s="7" t="inlineStr">
+    <row r="9" ht="210" customHeight="1">
+      <c r="A9" s="7" t="inlineStr">
         <is>
           <t>PIS</t>
         </is>
       </c>
-      <c r="B8" s="8" t="inlineStr">
-        <is>
-          <t>UNCATEGORIZED</t>
-        </is>
-      </c>
-      <c r="C8" s="8" t="inlineStr">
+      <c r="B9" s="8" t="inlineStr">
+        <is>
+          <t>UNCATEGORIZED</t>
+        </is>
+      </c>
+      <c r="C9" s="8" t="inlineStr">
         <is>
           <t>/v2_1_1.1/payments/v2_1_1.1/EEA.post.parameters</t>
         </is>
       </c>
-      <c r="D8" s="8" t="inlineStr">
+      <c r="D9" s="8" t="inlineStr">
         <is>
           <t xml:space="preserve">- $ref: '#/parameters/authorizationParam'
 - $ref: '#/parameters/acceptEncodingParam'
@@ -835,7 +866,7 @@
 </t>
         </is>
       </c>
-      <c r="E8" s="8" t="inlineStr">
+      <c r="E9" s="8" t="inlineStr">
         <is>
           <t xml:space="preserve">- $ref: '#/parameters/authorizationParam'
 - $ref: '#/parameters/acceptEncodingParam'
@@ -853,30 +884,30 @@
 </t>
         </is>
       </c>
-      <c r="F8" s="8" t="inlineStr">
+      <c r="F9" s="8" t="inlineStr">
         <is>
           <t>Added:
 • $ref: #/parameters/contentTypeParam</t>
         </is>
       </c>
     </row>
-    <row r="9" ht="60" customHeight="1">
-      <c r="A9" s="7" t="inlineStr">
+    <row r="10" ht="60" customHeight="1">
+      <c r="A10" s="7" t="inlineStr">
         <is>
           <t>PIS</t>
         </is>
       </c>
-      <c r="B9" s="8" t="inlineStr">
-        <is>
-          <t>UNCATEGORIZED</t>
-        </is>
-      </c>
-      <c r="C9" s="8" t="inlineStr">
+      <c r="B10" s="8" t="inlineStr">
+        <is>
+          <t>UNCATEGORIZED</t>
+        </is>
+      </c>
+      <c r="C10" s="8" t="inlineStr">
         <is>
           <t>/v2_1_1.1/payments/v2_1_1.1/EEA.post.responses.500</t>
         </is>
       </c>
-      <c r="D9" s="8" t="inlineStr">
+      <c r="D10" s="8" t="inlineStr">
         <is>
           <t xml:space="preserve">description: Internal Server Error
 schema:
@@ -884,8 +915,8 @@
 </t>
         </is>
       </c>
-      <c r="E9" s="8" t="inlineStr"/>
-      <c r="F9" s="8" t="inlineStr">
+      <c r="E10" s="8" t="inlineStr"/>
+      <c r="F10" s="8" t="inlineStr">
         <is>
           <t>Removed:
 • description: Internal Server Error
@@ -894,23 +925,23 @@
         </is>
       </c>
     </row>
-    <row r="10" ht="60" customHeight="1">
-      <c r="A10" s="7" t="inlineStr">
+    <row r="11" ht="60" customHeight="1">
+      <c r="A11" s="7" t="inlineStr">
         <is>
           <t>PIS</t>
         </is>
       </c>
-      <c r="B10" s="8" t="inlineStr">
-        <is>
-          <t>UNCATEGORIZED</t>
-        </is>
-      </c>
-      <c r="C10" s="8" t="inlineStr">
+      <c r="B11" s="8" t="inlineStr">
+        <is>
+          <t>UNCATEGORIZED</t>
+        </is>
+      </c>
+      <c r="C11" s="8" t="inlineStr">
         <is>
           <t>/v2_1_1.1/payments/v2_1_1.1/EEA.post.responses.503</t>
         </is>
       </c>
-      <c r="D10" s="8" t="inlineStr">
+      <c r="D11" s="8" t="inlineStr">
         <is>
           <t xml:space="preserve">description: Service Unavailable
 schema:
@@ -918,8 +949,8 @@
 </t>
         </is>
       </c>
-      <c r="E10" s="8" t="inlineStr"/>
-      <c r="F10" s="8" t="inlineStr">
+      <c r="E11" s="8" t="inlineStr"/>
+      <c r="F11" s="8" t="inlineStr">
         <is>
           <t>Removed:
 • description: Service Unavailable
@@ -928,24 +959,24 @@
         </is>
       </c>
     </row>
-    <row r="11" ht="60" customHeight="1">
-      <c r="A11" s="7" t="inlineStr">
+    <row r="12" ht="60" customHeight="1">
+      <c r="A12" s="7" t="inlineStr">
         <is>
           <t>PIS</t>
         </is>
       </c>
-      <c r="B11" s="8" t="inlineStr">
-        <is>
-          <t>UNCATEGORIZED</t>
-        </is>
-      </c>
-      <c r="C11" s="8" t="inlineStr">
+      <c r="B12" s="8" t="inlineStr">
+        <is>
+          <t>UNCATEGORIZED</t>
+        </is>
+      </c>
+      <c r="C12" s="8" t="inlineStr">
         <is>
           <t>/v2_1_1.1/payments/v2_1_1.1/EEA.post.responses.510</t>
         </is>
       </c>
-      <c r="D11" s="8" t="inlineStr"/>
-      <c r="E11" s="8" t="inlineStr">
+      <c r="D12" s="8" t="inlineStr"/>
+      <c r="E12" s="8" t="inlineStr">
         <is>
           <t xml:space="preserve">description: Internal Server Error
 schema:
@@ -953,7 +984,7 @@
 </t>
         </is>
       </c>
-      <c r="F11" s="8" t="inlineStr">
+      <c r="F12" s="8" t="inlineStr">
         <is>
           <t>Added:
 • description: Internal Server Error
@@ -962,23 +993,23 @@
         </is>
       </c>
     </row>
-    <row r="12" ht="75" customHeight="1">
-      <c r="A12" s="7" t="inlineStr">
+    <row r="13" ht="75" customHeight="1">
+      <c r="A13" s="7" t="inlineStr">
         <is>
           <t>PIS</t>
         </is>
       </c>
-      <c r="B12" s="8" t="inlineStr">
-        <is>
-          <t>UNCATEGORIZED</t>
-        </is>
-      </c>
-      <c r="C12" s="8" t="inlineStr">
+      <c r="B13" s="8" t="inlineStr">
+        <is>
+          <t>UNCATEGORIZED</t>
+        </is>
+      </c>
+      <c r="C13" s="8" t="inlineStr">
         <is>
           <t>/v2_1_1.1/payments/v2_1_1.1/EEA.post.security</t>
         </is>
       </c>
-      <c r="D12" s="8" t="inlineStr">
+      <c r="D13" s="8" t="inlineStr">
         <is>
           <t xml:space="preserve">- xs2a_auth_aspsp:
   - pis
@@ -987,14 +1018,14 @@
 </t>
         </is>
       </c>
-      <c r="E12" s="8" t="inlineStr">
+      <c r="E13" s="8" t="inlineStr">
         <is>
           <t xml:space="preserve">- xs2a_auth_decoupled:
   - pis
 </t>
         </is>
       </c>
-      <c r="F12" s="8" t="inlineStr">
+      <c r="F13" s="8" t="inlineStr">
         <is>
           <t>Removed:
 • xs2a_auth_aspsp:
@@ -1002,54 +1033,54 @@
         </is>
       </c>
     </row>
-    <row r="13" ht="45" customHeight="1">
-      <c r="A13" s="7" t="inlineStr">
+    <row r="14" ht="45" customHeight="1">
+      <c r="A14" s="7" t="inlineStr">
         <is>
           <t>PIS</t>
         </is>
       </c>
-      <c r="B13" s="8" t="inlineStr">
-        <is>
-          <t>UNCATEGORIZED</t>
-        </is>
-      </c>
-      <c r="C13" s="8" t="inlineStr">
+      <c r="B14" s="8" t="inlineStr">
+        <is>
+          <t>UNCATEGORIZED</t>
+        </is>
+      </c>
+      <c r="C14" s="8" t="inlineStr">
         <is>
           <t>/v2_1_1.1/payments/v2_1_1.1/nonEEA.x-swagger-router-controller</t>
         </is>
       </c>
-      <c r="D13" s="8" t="inlineStr">
+      <c r="D14" s="8" t="inlineStr">
         <is>
           <t xml:space="preserve">pis
 ...
 </t>
         </is>
       </c>
-      <c r="E13" s="8" t="inlineStr"/>
-      <c r="F13" s="8" t="inlineStr">
+      <c r="E14" s="8" t="inlineStr"/>
+      <c r="F14" s="8" t="inlineStr">
         <is>
           <t>Removed:
 • pis</t>
         </is>
       </c>
     </row>
-    <row r="14" ht="210" customHeight="1">
-      <c r="A14" s="7" t="inlineStr">
+    <row r="15" ht="210" customHeight="1">
+      <c r="A15" s="7" t="inlineStr">
         <is>
           <t>PIS</t>
         </is>
       </c>
-      <c r="B14" s="8" t="inlineStr">
-        <is>
-          <t>UNCATEGORIZED</t>
-        </is>
-      </c>
-      <c r="C14" s="8" t="inlineStr">
+      <c r="B15" s="8" t="inlineStr">
+        <is>
+          <t>UNCATEGORIZED</t>
+        </is>
+      </c>
+      <c r="C15" s="8" t="inlineStr">
         <is>
           <t>/v2_1_1.1/payments/v2_1_1.1/nonEEA.post.parameters</t>
         </is>
       </c>
-      <c r="D14" s="8" t="inlineStr">
+      <c r="D15" s="8" t="inlineStr">
         <is>
           <t xml:space="preserve">- $ref: '#/parameters/authorizationParam'
 - $ref: '#/parameters/acceptEncodingParam'
@@ -1066,7 +1097,7 @@
 </t>
         </is>
       </c>
-      <c r="E14" s="8" t="inlineStr">
+      <c r="E15" s="8" t="inlineStr">
         <is>
           <t xml:space="preserve">- $ref: '#/parameters/authorizationParam'
 - $ref: '#/parameters/acceptEncodingParam'
@@ -1084,30 +1115,30 @@
 </t>
         </is>
       </c>
-      <c r="F14" s="8" t="inlineStr">
+      <c r="F15" s="8" t="inlineStr">
         <is>
           <t>Added:
 • $ref: #/parameters/contentTypeParam</t>
         </is>
       </c>
     </row>
-    <row r="15" ht="60" customHeight="1">
-      <c r="A15" s="7" t="inlineStr">
+    <row r="16" ht="60" customHeight="1">
+      <c r="A16" s="7" t="inlineStr">
         <is>
           <t>PIS</t>
         </is>
       </c>
-      <c r="B15" s="8" t="inlineStr">
-        <is>
-          <t>UNCATEGORIZED</t>
-        </is>
-      </c>
-      <c r="C15" s="8" t="inlineStr">
+      <c r="B16" s="8" t="inlineStr">
+        <is>
+          <t>UNCATEGORIZED</t>
+        </is>
+      </c>
+      <c r="C16" s="8" t="inlineStr">
         <is>
           <t>/v2_1_1.1/payments/v2_1_1.1/nonEEA.post.responses.500</t>
         </is>
       </c>
-      <c r="D15" s="8" t="inlineStr">
+      <c r="D16" s="8" t="inlineStr">
         <is>
           <t xml:space="preserve">description: Internal Server Error
 schema:
@@ -1115,8 +1146,8 @@
 </t>
         </is>
       </c>
-      <c r="E15" s="8" t="inlineStr"/>
-      <c r="F15" s="8" t="inlineStr">
+      <c r="E16" s="8" t="inlineStr"/>
+      <c r="F16" s="8" t="inlineStr">
         <is>
           <t>Removed:
 • description: Internal Server Error
@@ -1125,23 +1156,23 @@
         </is>
       </c>
     </row>
-    <row r="16" ht="60" customHeight="1">
-      <c r="A16" s="7" t="inlineStr">
+    <row r="17" ht="60" customHeight="1">
+      <c r="A17" s="7" t="inlineStr">
         <is>
           <t>PIS</t>
         </is>
       </c>
-      <c r="B16" s="8" t="inlineStr">
-        <is>
-          <t>UNCATEGORIZED</t>
-        </is>
-      </c>
-      <c r="C16" s="8" t="inlineStr">
+      <c r="B17" s="8" t="inlineStr">
+        <is>
+          <t>UNCATEGORIZED</t>
+        </is>
+      </c>
+      <c r="C17" s="8" t="inlineStr">
         <is>
           <t>/v2_1_1.1/payments/v2_1_1.1/nonEEA.post.responses.503</t>
         </is>
       </c>
-      <c r="D16" s="8" t="inlineStr">
+      <c r="D17" s="8" t="inlineStr">
         <is>
           <t xml:space="preserve">description: Service Unavailable
 schema:
@@ -1149,8 +1180,8 @@
 </t>
         </is>
       </c>
-      <c r="E16" s="8" t="inlineStr"/>
-      <c r="F16" s="8" t="inlineStr">
+      <c r="E17" s="8" t="inlineStr"/>
+      <c r="F17" s="8" t="inlineStr">
         <is>
           <t>Removed:
 • description: Service Unavailable
@@ -1159,24 +1190,24 @@
         </is>
       </c>
     </row>
-    <row r="17" ht="60" customHeight="1">
-      <c r="A17" s="7" t="inlineStr">
+    <row r="18" ht="60" customHeight="1">
+      <c r="A18" s="7" t="inlineStr">
         <is>
           <t>PIS</t>
         </is>
       </c>
-      <c r="B17" s="8" t="inlineStr">
-        <is>
-          <t>UNCATEGORIZED</t>
-        </is>
-      </c>
-      <c r="C17" s="8" t="inlineStr">
+      <c r="B18" s="8" t="inlineStr">
+        <is>
+          <t>UNCATEGORIZED</t>
+        </is>
+      </c>
+      <c r="C18" s="8" t="inlineStr">
         <is>
           <t>/v2_1_1.1/payments/v2_1_1.1/nonEEA.post.responses.510</t>
         </is>
       </c>
-      <c r="D17" s="8" t="inlineStr"/>
-      <c r="E17" s="8" t="inlineStr">
+      <c r="D18" s="8" t="inlineStr"/>
+      <c r="E18" s="8" t="inlineStr">
         <is>
           <t xml:space="preserve">description: Internal Server Error
 schema:
@@ -1184,7 +1215,7 @@
 </t>
         </is>
       </c>
-      <c r="F17" s="8" t="inlineStr">
+      <c r="F18" s="8" t="inlineStr">
         <is>
           <t>Added:
 • description: Internal Server Error
@@ -1193,23 +1224,23 @@
         </is>
       </c>
     </row>
-    <row r="18" ht="75" customHeight="1">
-      <c r="A18" s="7" t="inlineStr">
+    <row r="19" ht="75" customHeight="1">
+      <c r="A19" s="7" t="inlineStr">
         <is>
           <t>PIS</t>
         </is>
       </c>
-      <c r="B18" s="8" t="inlineStr">
-        <is>
-          <t>UNCATEGORIZED</t>
-        </is>
-      </c>
-      <c r="C18" s="8" t="inlineStr">
+      <c r="B19" s="8" t="inlineStr">
+        <is>
+          <t>UNCATEGORIZED</t>
+        </is>
+      </c>
+      <c r="C19" s="8" t="inlineStr">
         <is>
           <t>/v2_1_1.1/payments/v2_1_1.1/nonEEA.post.security</t>
         </is>
       </c>
-      <c r="D18" s="8" t="inlineStr">
+      <c r="D19" s="8" t="inlineStr">
         <is>
           <t xml:space="preserve">- xs2a_auth_aspsp:
   - pis
@@ -1218,14 +1249,14 @@
 </t>
         </is>
       </c>
-      <c r="E18" s="8" t="inlineStr">
+      <c r="E19" s="8" t="inlineStr">
         <is>
           <t xml:space="preserve">- xs2a_auth_decoupled:
   - pis
 </t>
         </is>
       </c>
-      <c r="F18" s="8" t="inlineStr">
+      <c r="F19" s="8" t="inlineStr">
         <is>
           <t>Removed:
 • xs2a_auth_aspsp:
@@ -1233,54 +1264,54 @@
         </is>
       </c>
     </row>
-    <row r="19" ht="45" customHeight="1">
-      <c r="A19" s="7" t="inlineStr">
+    <row r="20" ht="45" customHeight="1">
+      <c r="A20" s="7" t="inlineStr">
         <is>
           <t>PIS</t>
         </is>
       </c>
-      <c r="B19" s="8" t="inlineStr">
-        <is>
-          <t>UNCATEGORIZED</t>
-        </is>
-      </c>
-      <c r="C19" s="8" t="inlineStr">
+      <c r="B20" s="8" t="inlineStr">
+        <is>
+          <t>UNCATEGORIZED</t>
+        </is>
+      </c>
+      <c r="C20" s="8" t="inlineStr">
         <is>
           <t>/v2_1_1.1/payments/v2_1_1.1/tax.x-swagger-router-controller</t>
         </is>
       </c>
-      <c r="D19" s="8" t="inlineStr">
+      <c r="D20" s="8" t="inlineStr">
         <is>
           <t xml:space="preserve">pis
 ...
 </t>
         </is>
       </c>
-      <c r="E19" s="8" t="inlineStr"/>
-      <c r="F19" s="8" t="inlineStr">
+      <c r="E20" s="8" t="inlineStr"/>
+      <c r="F20" s="8" t="inlineStr">
         <is>
           <t>Removed:
 • pis</t>
         </is>
       </c>
     </row>
-    <row r="20" ht="210" customHeight="1">
-      <c r="A20" s="7" t="inlineStr">
+    <row r="21" ht="210" customHeight="1">
+      <c r="A21" s="7" t="inlineStr">
         <is>
           <t>PIS</t>
         </is>
       </c>
-      <c r="B20" s="8" t="inlineStr">
-        <is>
-          <t>UNCATEGORIZED</t>
-        </is>
-      </c>
-      <c r="C20" s="8" t="inlineStr">
+      <c r="B21" s="8" t="inlineStr">
+        <is>
+          <t>UNCATEGORIZED</t>
+        </is>
+      </c>
+      <c r="C21" s="8" t="inlineStr">
         <is>
           <t>/v2_1_1.1/payments/v2_1_1.1/tax.post.parameters</t>
         </is>
       </c>
-      <c r="D20" s="8" t="inlineStr">
+      <c r="D21" s="8" t="inlineStr">
         <is>
           <t xml:space="preserve">- $ref: '#/parameters/authorizationParam'
 - $ref: '#/parameters/acceptEncodingParam'
@@ -1297,7 +1328,7 @@
 </t>
         </is>
       </c>
-      <c r="E20" s="8" t="inlineStr">
+      <c r="E21" s="8" t="inlineStr">
         <is>
           <t xml:space="preserve">- $ref: '#/parameters/authorizationParam'
 - $ref: '#/parameters/acceptEncodingParam'
@@ -1315,30 +1346,30 @@
 </t>
         </is>
       </c>
-      <c r="F20" s="8" t="inlineStr">
+      <c r="F21" s="8" t="inlineStr">
         <is>
           <t>Added:
 • $ref: #/parameters/contentTypeParam</t>
         </is>
       </c>
     </row>
-    <row r="21" ht="60" customHeight="1">
-      <c r="A21" s="7" t="inlineStr">
+    <row r="22" ht="60" customHeight="1">
+      <c r="A22" s="7" t="inlineStr">
         <is>
           <t>PIS</t>
         </is>
       </c>
-      <c r="B21" s="8" t="inlineStr">
-        <is>
-          <t>UNCATEGORIZED</t>
-        </is>
-      </c>
-      <c r="C21" s="8" t="inlineStr">
+      <c r="B22" s="8" t="inlineStr">
+        <is>
+          <t>UNCATEGORIZED</t>
+        </is>
+      </c>
+      <c r="C22" s="8" t="inlineStr">
         <is>
           <t>/v2_1_1.1/payments/v2_1_1.1/tax.post.responses.500</t>
         </is>
       </c>
-      <c r="D21" s="8" t="inlineStr">
+      <c r="D22" s="8" t="inlineStr">
         <is>
           <t xml:space="preserve">description: Internal Server Error
 schema:
@@ -1346,8 +1377,8 @@
 </t>
         </is>
       </c>
-      <c r="E21" s="8" t="inlineStr"/>
-      <c r="F21" s="8" t="inlineStr">
+      <c r="E22" s="8" t="inlineStr"/>
+      <c r="F22" s="8" t="inlineStr">
         <is>
           <t>Removed:
 • description: Internal Server Error
@@ -1356,23 +1387,23 @@
         </is>
       </c>
     </row>
-    <row r="22" ht="60" customHeight="1">
-      <c r="A22" s="7" t="inlineStr">
+    <row r="23" ht="60" customHeight="1">
+      <c r="A23" s="7" t="inlineStr">
         <is>
           <t>PIS</t>
         </is>
       </c>
-      <c r="B22" s="8" t="inlineStr">
-        <is>
-          <t>UNCATEGORIZED</t>
-        </is>
-      </c>
-      <c r="C22" s="8" t="inlineStr">
+      <c r="B23" s="8" t="inlineStr">
+        <is>
+          <t>UNCATEGORIZED</t>
+        </is>
+      </c>
+      <c r="C23" s="8" t="inlineStr">
         <is>
           <t>/v2_1_1.1/payments/v2_1_1.1/tax.post.responses.503</t>
         </is>
       </c>
-      <c r="D22" s="8" t="inlineStr">
+      <c r="D23" s="8" t="inlineStr">
         <is>
           <t xml:space="preserve">description: Service Unavailable
 schema:
@@ -1380,8 +1411,8 @@
 </t>
         </is>
       </c>
-      <c r="E22" s="8" t="inlineStr"/>
-      <c r="F22" s="8" t="inlineStr">
+      <c r="E23" s="8" t="inlineStr"/>
+      <c r="F23" s="8" t="inlineStr">
         <is>
           <t>Removed:
 • description: Service Unavailable
@@ -1390,24 +1421,24 @@
         </is>
       </c>
     </row>
-    <row r="23" ht="60" customHeight="1">
-      <c r="A23" s="7" t="inlineStr">
+    <row r="24" ht="60" customHeight="1">
+      <c r="A24" s="7" t="inlineStr">
         <is>
           <t>PIS</t>
         </is>
       </c>
-      <c r="B23" s="8" t="inlineStr">
-        <is>
-          <t>UNCATEGORIZED</t>
-        </is>
-      </c>
-      <c r="C23" s="8" t="inlineStr">
+      <c r="B24" s="8" t="inlineStr">
+        <is>
+          <t>UNCATEGORIZED</t>
+        </is>
+      </c>
+      <c r="C24" s="8" t="inlineStr">
         <is>
           <t>/v2_1_1.1/payments/v2_1_1.1/tax.post.responses.510</t>
         </is>
       </c>
-      <c r="D23" s="8" t="inlineStr"/>
-      <c r="E23" s="8" t="inlineStr">
+      <c r="D24" s="8" t="inlineStr"/>
+      <c r="E24" s="8" t="inlineStr">
         <is>
           <t xml:space="preserve">description: Internal Server Error
 schema:
@@ -1415,7 +1446,7 @@
 </t>
         </is>
       </c>
-      <c r="F23" s="8" t="inlineStr">
+      <c r="F24" s="8" t="inlineStr">
         <is>
           <t>Added:
 • description: Internal Server Error
@@ -1424,23 +1455,23 @@
         </is>
       </c>
     </row>
-    <row r="24" ht="75" customHeight="1">
-      <c r="A24" s="7" t="inlineStr">
+    <row r="25" ht="75" customHeight="1">
+      <c r="A25" s="7" t="inlineStr">
         <is>
           <t>PIS</t>
         </is>
       </c>
-      <c r="B24" s="8" t="inlineStr">
-        <is>
-          <t>UNCATEGORIZED</t>
-        </is>
-      </c>
-      <c r="C24" s="8" t="inlineStr">
+      <c r="B25" s="8" t="inlineStr">
+        <is>
+          <t>UNCATEGORIZED</t>
+        </is>
+      </c>
+      <c r="C25" s="8" t="inlineStr">
         <is>
           <t>/v2_1_1.1/payments/v2_1_1.1/tax.post.security</t>
         </is>
       </c>
-      <c r="D24" s="8" t="inlineStr">
+      <c r="D25" s="8" t="inlineStr">
         <is>
           <t xml:space="preserve">- xs2a_auth_aspsp:
   - pis
@@ -1449,14 +1480,14 @@
 </t>
         </is>
       </c>
-      <c r="E24" s="8" t="inlineStr">
+      <c r="E25" s="8" t="inlineStr">
         <is>
           <t xml:space="preserve">- xs2a_auth_decoupled:
   - pis
 </t>
         </is>
       </c>
-      <c r="F24" s="8" t="inlineStr">
+      <c r="F25" s="8" t="inlineStr">
         <is>
           <t>Removed:
 • xs2a_auth_aspsp:
@@ -1464,54 +1495,54 @@
         </is>
       </c>
     </row>
-    <row r="25" ht="45" customHeight="1">
-      <c r="A25" s="7" t="inlineStr">
+    <row r="26" ht="45" customHeight="1">
+      <c r="A26" s="7" t="inlineStr">
         <is>
           <t>PIS</t>
         </is>
       </c>
-      <c r="B25" s="8" t="inlineStr">
-        <is>
-          <t>UNCATEGORIZED</t>
-        </is>
-      </c>
-      <c r="C25" s="8" t="inlineStr">
+      <c r="B26" s="8" t="inlineStr">
+        <is>
+          <t>UNCATEGORIZED</t>
+        </is>
+      </c>
+      <c r="C26" s="8" t="inlineStr">
         <is>
           <t>/v2_1_1.1/payments/v2_1_1.1/bundle.x-swagger-router-controller</t>
         </is>
       </c>
-      <c r="D25" s="8" t="inlineStr">
+      <c r="D26" s="8" t="inlineStr">
         <is>
           <t xml:space="preserve">pis
 ...
 </t>
         </is>
       </c>
-      <c r="E25" s="8" t="inlineStr"/>
-      <c r="F25" s="8" t="inlineStr">
+      <c r="E26" s="8" t="inlineStr"/>
+      <c r="F26" s="8" t="inlineStr">
         <is>
           <t>Removed:
 • pis</t>
         </is>
       </c>
     </row>
-    <row r="26" ht="210" customHeight="1">
-      <c r="A26" s="7" t="inlineStr">
+    <row r="27" ht="210" customHeight="1">
+      <c r="A27" s="7" t="inlineStr">
         <is>
           <t>PIS</t>
         </is>
       </c>
-      <c r="B26" s="8" t="inlineStr">
-        <is>
-          <t>UNCATEGORIZED</t>
-        </is>
-      </c>
-      <c r="C26" s="8" t="inlineStr">
+      <c r="B27" s="8" t="inlineStr">
+        <is>
+          <t>UNCATEGORIZED</t>
+        </is>
+      </c>
+      <c r="C27" s="8" t="inlineStr">
         <is>
           <t>/v2_1_1.1/payments/v2_1_1.1/bundle.post.parameters</t>
         </is>
       </c>
-      <c r="D26" s="8" t="inlineStr">
+      <c r="D27" s="8" t="inlineStr">
         <is>
           <t xml:space="preserve">- $ref: '#/parameters/authorizationParam'
 - $ref: '#/parameters/acceptEncodingParam'
@@ -1528,7 +1559,7 @@
 </t>
         </is>
       </c>
-      <c r="E26" s="8" t="inlineStr">
+      <c r="E27" s="8" t="inlineStr">
         <is>
           <t xml:space="preserve">- $ref: '#/parameters/authorizationParam'
 - $ref: '#/parameters/acceptEncodingParam'
@@ -1546,30 +1577,30 @@
 </t>
         </is>
       </c>
-      <c r="F26" s="8" t="inlineStr">
+      <c r="F27" s="8" t="inlineStr">
         <is>
           <t>Added:
 • $ref: #/parameters/contentTypeParam</t>
         </is>
       </c>
     </row>
-    <row r="27" ht="60" customHeight="1">
-      <c r="A27" s="7" t="inlineStr">
+    <row r="28" ht="60" customHeight="1">
+      <c r="A28" s="7" t="inlineStr">
         <is>
           <t>PIS</t>
         </is>
       </c>
-      <c r="B27" s="8" t="inlineStr">
-        <is>
-          <t>UNCATEGORIZED</t>
-        </is>
-      </c>
-      <c r="C27" s="8" t="inlineStr">
+      <c r="B28" s="8" t="inlineStr">
+        <is>
+          <t>UNCATEGORIZED</t>
+        </is>
+      </c>
+      <c r="C28" s="8" t="inlineStr">
         <is>
           <t>/v2_1_1.1/payments/v2_1_1.1/bundle.post.responses.500</t>
         </is>
       </c>
-      <c r="D27" s="8" t="inlineStr">
+      <c r="D28" s="8" t="inlineStr">
         <is>
           <t xml:space="preserve">description: Internal Server Error
 schema:
@@ -1577,8 +1608,8 @@
 </t>
         </is>
       </c>
-      <c r="E27" s="8" t="inlineStr"/>
-      <c r="F27" s="8" t="inlineStr">
+      <c r="E28" s="8" t="inlineStr"/>
+      <c r="F28" s="8" t="inlineStr">
         <is>
           <t>Removed:
 • description: Internal Server Error
@@ -1587,23 +1618,23 @@
         </is>
       </c>
     </row>
-    <row r="28" ht="60" customHeight="1">
-      <c r="A28" s="7" t="inlineStr">
+    <row r="29" ht="60" customHeight="1">
+      <c r="A29" s="7" t="inlineStr">
         <is>
           <t>PIS</t>
         </is>
       </c>
-      <c r="B28" s="8" t="inlineStr">
-        <is>
-          <t>UNCATEGORIZED</t>
-        </is>
-      </c>
-      <c r="C28" s="8" t="inlineStr">
+      <c r="B29" s="8" t="inlineStr">
+        <is>
+          <t>UNCATEGORIZED</t>
+        </is>
+      </c>
+      <c r="C29" s="8" t="inlineStr">
         <is>
           <t>/v2_1_1.1/payments/v2_1_1.1/bundle.post.responses.503</t>
         </is>
       </c>
-      <c r="D28" s="8" t="inlineStr">
+      <c r="D29" s="8" t="inlineStr">
         <is>
           <t xml:space="preserve">description: Service Unavailable
 schema:
@@ -1611,8 +1642,8 @@
 </t>
         </is>
       </c>
-      <c r="E28" s="8" t="inlineStr"/>
-      <c r="F28" s="8" t="inlineStr">
+      <c r="E29" s="8" t="inlineStr"/>
+      <c r="F29" s="8" t="inlineStr">
         <is>
           <t>Removed:
 • description: Service Unavailable
@@ -1621,24 +1652,24 @@
         </is>
       </c>
     </row>
-    <row r="29" ht="60" customHeight="1">
-      <c r="A29" s="7" t="inlineStr">
+    <row r="30" ht="60" customHeight="1">
+      <c r="A30" s="7" t="inlineStr">
         <is>
           <t>PIS</t>
         </is>
       </c>
-      <c r="B29" s="8" t="inlineStr">
-        <is>
-          <t>UNCATEGORIZED</t>
-        </is>
-      </c>
-      <c r="C29" s="8" t="inlineStr">
+      <c r="B30" s="8" t="inlineStr">
+        <is>
+          <t>UNCATEGORIZED</t>
+        </is>
+      </c>
+      <c r="C30" s="8" t="inlineStr">
         <is>
           <t>/v2_1_1.1/payments/v2_1_1.1/bundle.post.responses.510</t>
         </is>
       </c>
-      <c r="D29" s="8" t="inlineStr"/>
-      <c r="E29" s="8" t="inlineStr">
+      <c r="D30" s="8" t="inlineStr"/>
+      <c r="E30" s="8" t="inlineStr">
         <is>
           <t xml:space="preserve">description: Internal Server Error
 schema:
@@ -1646,7 +1677,7 @@
 </t>
         </is>
       </c>
-      <c r="F29" s="8" t="inlineStr">
+      <c r="F30" s="8" t="inlineStr">
         <is>
           <t>Added:
 • description: Internal Server Error
@@ -1655,23 +1686,23 @@
         </is>
       </c>
     </row>
-    <row r="30" ht="75" customHeight="1">
-      <c r="A30" s="7" t="inlineStr">
+    <row r="31" ht="75" customHeight="1">
+      <c r="A31" s="7" t="inlineStr">
         <is>
           <t>PIS</t>
         </is>
       </c>
-      <c r="B30" s="8" t="inlineStr">
-        <is>
-          <t>UNCATEGORIZED</t>
-        </is>
-      </c>
-      <c r="C30" s="8" t="inlineStr">
+      <c r="B31" s="8" t="inlineStr">
+        <is>
+          <t>UNCATEGORIZED</t>
+        </is>
+      </c>
+      <c r="C31" s="8" t="inlineStr">
         <is>
           <t>/v2_1_1.1/payments/v2_1_1.1/bundle.post.security</t>
         </is>
       </c>
-      <c r="D30" s="8" t="inlineStr">
+      <c r="D31" s="8" t="inlineStr">
         <is>
           <t xml:space="preserve">- xs2a_auth_aspsp:
   - pis
@@ -1680,14 +1711,14 @@
 </t>
         </is>
       </c>
-      <c r="E30" s="8" t="inlineStr">
+      <c r="E31" s="8" t="inlineStr">
         <is>
           <t xml:space="preserve">- xs2a_auth_decoupled:
   - pis
 </t>
         </is>
       </c>
-      <c r="F30" s="8" t="inlineStr">
+      <c r="F31" s="8" t="inlineStr">
         <is>
           <t>Removed:
 • xs2a_auth_aspsp:
@@ -1695,54 +1726,54 @@
         </is>
       </c>
     </row>
-    <row r="31" ht="45" customHeight="1">
-      <c r="A31" s="7" t="inlineStr">
+    <row r="32" ht="45" customHeight="1">
+      <c r="A32" s="7" t="inlineStr">
         <is>
           <t>PIS</t>
         </is>
       </c>
-      <c r="B31" s="8" t="inlineStr">
-        <is>
-          <t>UNCATEGORIZED</t>
-        </is>
-      </c>
-      <c r="C31" s="8" t="inlineStr">
+      <c r="B32" s="8" t="inlineStr">
+        <is>
+          <t>UNCATEGORIZED</t>
+        </is>
+      </c>
+      <c r="C32" s="8" t="inlineStr">
         <is>
           <t>/v2_1_1.1/payments/v2_1_1.1/recurring.x-swagger-router-controller</t>
         </is>
       </c>
-      <c r="D31" s="8" t="inlineStr">
+      <c r="D32" s="8" t="inlineStr">
         <is>
           <t xml:space="preserve">pis
 ...
 </t>
         </is>
       </c>
-      <c r="E31" s="8" t="inlineStr"/>
-      <c r="F31" s="8" t="inlineStr">
+      <c r="E32" s="8" t="inlineStr"/>
+      <c r="F32" s="8" t="inlineStr">
         <is>
           <t>Removed:
 • pis</t>
         </is>
       </c>
     </row>
-    <row r="32" ht="210" customHeight="1">
-      <c r="A32" s="7" t="inlineStr">
+    <row r="33" ht="210" customHeight="1">
+      <c r="A33" s="7" t="inlineStr">
         <is>
           <t>PIS</t>
         </is>
       </c>
-      <c r="B32" s="8" t="inlineStr">
-        <is>
-          <t>UNCATEGORIZED</t>
-        </is>
-      </c>
-      <c r="C32" s="8" t="inlineStr">
+      <c r="B33" s="8" t="inlineStr">
+        <is>
+          <t>UNCATEGORIZED</t>
+        </is>
+      </c>
+      <c r="C33" s="8" t="inlineStr">
         <is>
           <t>/v2_1_1.1/payments/v2_1_1.1/recurring.post.parameters</t>
         </is>
       </c>
-      <c r="D32" s="8" t="inlineStr">
+      <c r="D33" s="8" t="inlineStr">
         <is>
           <t xml:space="preserve">- $ref: '#/parameters/authorizationParam'
 - $ref: '#/parameters/acceptEncodingParam'
@@ -1759,7 +1790,7 @@
 </t>
         </is>
       </c>
-      <c r="E32" s="8" t="inlineStr">
+      <c r="E33" s="8" t="inlineStr">
         <is>
           <t xml:space="preserve">- $ref: '#/parameters/authorizationParam'
 - $ref: '#/parameters/acceptEncodingParam'
@@ -1777,30 +1808,30 @@
 </t>
         </is>
       </c>
-      <c r="F32" s="8" t="inlineStr">
+      <c r="F33" s="8" t="inlineStr">
         <is>
           <t>Added:
 • $ref: #/parameters/contentTypeParam</t>
         </is>
       </c>
     </row>
-    <row r="33" ht="60" customHeight="1">
-      <c r="A33" s="7" t="inlineStr">
+    <row r="34" ht="60" customHeight="1">
+      <c r="A34" s="7" t="inlineStr">
         <is>
           <t>PIS</t>
         </is>
       </c>
-      <c r="B33" s="8" t="inlineStr">
-        <is>
-          <t>UNCATEGORIZED</t>
-        </is>
-      </c>
-      <c r="C33" s="8" t="inlineStr">
+      <c r="B34" s="8" t="inlineStr">
+        <is>
+          <t>UNCATEGORIZED</t>
+        </is>
+      </c>
+      <c r="C34" s="8" t="inlineStr">
         <is>
           <t>/v2_1_1.1/payments/v2_1_1.1/recurring.post.responses.500</t>
         </is>
       </c>
-      <c r="D33" s="8" t="inlineStr">
+      <c r="D34" s="8" t="inlineStr">
         <is>
           <t xml:space="preserve">description: Internal Server Error
 schema:
@@ -1808,8 +1839,8 @@
 </t>
         </is>
       </c>
-      <c r="E33" s="8" t="inlineStr"/>
-      <c r="F33" s="8" t="inlineStr">
+      <c r="E34" s="8" t="inlineStr"/>
+      <c r="F34" s="8" t="inlineStr">
         <is>
           <t>Removed:
 • description: Internal Server Error
@@ -1818,23 +1849,23 @@
         </is>
       </c>
     </row>
-    <row r="34" ht="60" customHeight="1">
-      <c r="A34" s="7" t="inlineStr">
+    <row r="35" ht="60" customHeight="1">
+      <c r="A35" s="7" t="inlineStr">
         <is>
           <t>PIS</t>
         </is>
       </c>
-      <c r="B34" s="8" t="inlineStr">
-        <is>
-          <t>UNCATEGORIZED</t>
-        </is>
-      </c>
-      <c r="C34" s="8" t="inlineStr">
+      <c r="B35" s="8" t="inlineStr">
+        <is>
+          <t>UNCATEGORIZED</t>
+        </is>
+      </c>
+      <c r="C35" s="8" t="inlineStr">
         <is>
           <t>/v2_1_1.1/payments/v2_1_1.1/recurring.post.responses.503</t>
         </is>
       </c>
-      <c r="D34" s="8" t="inlineStr">
+      <c r="D35" s="8" t="inlineStr">
         <is>
           <t xml:space="preserve">description: Service Unavailable
 schema:
@@ -1842,8 +1873,8 @@
 </t>
         </is>
       </c>
-      <c r="E34" s="8" t="inlineStr"/>
-      <c r="F34" s="8" t="inlineStr">
+      <c r="E35" s="8" t="inlineStr"/>
+      <c r="F35" s="8" t="inlineStr">
         <is>
           <t>Removed:
 • description: Service Unavailable
@@ -1852,24 +1883,24 @@
         </is>
       </c>
     </row>
-    <row r="35" ht="60" customHeight="1">
-      <c r="A35" s="7" t="inlineStr">
+    <row r="36" ht="60" customHeight="1">
+      <c r="A36" s="7" t="inlineStr">
         <is>
           <t>PIS</t>
         </is>
       </c>
-      <c r="B35" s="8" t="inlineStr">
-        <is>
-          <t>UNCATEGORIZED</t>
-        </is>
-      </c>
-      <c r="C35" s="8" t="inlineStr">
+      <c r="B36" s="8" t="inlineStr">
+        <is>
+          <t>UNCATEGORIZED</t>
+        </is>
+      </c>
+      <c r="C36" s="8" t="inlineStr">
         <is>
           <t>/v2_1_1.1/payments/v2_1_1.1/recurring.post.responses.510</t>
         </is>
       </c>
-      <c r="D35" s="8" t="inlineStr"/>
-      <c r="E35" s="8" t="inlineStr">
+      <c r="D36" s="8" t="inlineStr"/>
+      <c r="E36" s="8" t="inlineStr">
         <is>
           <t xml:space="preserve">description: Internal Server Error
 schema:
@@ -1877,7 +1908,7 @@
 </t>
         </is>
       </c>
-      <c r="F35" s="8" t="inlineStr">
+      <c r="F36" s="8" t="inlineStr">
         <is>
           <t>Added:
 • description: Internal Server Error
@@ -1886,23 +1917,23 @@
         </is>
       </c>
     </row>
-    <row r="36" ht="75" customHeight="1">
-      <c r="A36" s="7" t="inlineStr">
+    <row r="37" ht="75" customHeight="1">
+      <c r="A37" s="7" t="inlineStr">
         <is>
           <t>PIS</t>
         </is>
       </c>
-      <c r="B36" s="8" t="inlineStr">
-        <is>
-          <t>UNCATEGORIZED</t>
-        </is>
-      </c>
-      <c r="C36" s="8" t="inlineStr">
+      <c r="B37" s="8" t="inlineStr">
+        <is>
+          <t>UNCATEGORIZED</t>
+        </is>
+      </c>
+      <c r="C37" s="8" t="inlineStr">
         <is>
           <t>/v2_1_1.1/payments/v2_1_1.1/recurring.post.security</t>
         </is>
       </c>
-      <c r="D36" s="8" t="inlineStr">
+      <c r="D37" s="8" t="inlineStr">
         <is>
           <t xml:space="preserve">- xs2a_auth_aspsp:
   - pis
@@ -1911,14 +1942,14 @@
 </t>
         </is>
       </c>
-      <c r="E36" s="8" t="inlineStr">
+      <c r="E37" s="8" t="inlineStr">
         <is>
           <t xml:space="preserve">- xs2a_auth_decoupled:
   - pis
 </t>
         </is>
       </c>
-      <c r="F36" s="8" t="inlineStr">
+      <c r="F37" s="8" t="inlineStr">
         <is>
           <t>Removed:
 • xs2a_auth_aspsp:
@@ -1926,54 +1957,54 @@
         </is>
       </c>
     </row>
-    <row r="37" ht="45" customHeight="1">
-      <c r="A37" s="7" t="inlineStr">
+    <row r="38" ht="45" customHeight="1">
+      <c r="A38" s="7" t="inlineStr">
         <is>
           <t>PIS</t>
         </is>
       </c>
-      <c r="B37" s="8" t="inlineStr">
-        <is>
-          <t>UNCATEGORIZED</t>
-        </is>
-      </c>
-      <c r="C37" s="8" t="inlineStr">
+      <c r="B38" s="8" t="inlineStr">
+        <is>
+          <t>UNCATEGORIZED</t>
+        </is>
+      </c>
+      <c r="C38" s="8" t="inlineStr">
         <is>
           <t>/v2_1_1.1/payments/v2_1_1.1/getPayment.x-swagger-router-controller</t>
         </is>
       </c>
-      <c r="D37" s="8" t="inlineStr">
+      <c r="D38" s="8" t="inlineStr">
         <is>
           <t xml:space="preserve">pis
 ...
 </t>
         </is>
       </c>
-      <c r="E37" s="8" t="inlineStr"/>
-      <c r="F37" s="8" t="inlineStr">
+      <c r="E38" s="8" t="inlineStr"/>
+      <c r="F38" s="8" t="inlineStr">
         <is>
           <t>Removed:
 • pis</t>
         </is>
       </c>
     </row>
-    <row r="38" ht="210" customHeight="1">
-      <c r="A38" s="7" t="inlineStr">
+    <row r="39" ht="210" customHeight="1">
+      <c r="A39" s="7" t="inlineStr">
         <is>
           <t>PIS</t>
         </is>
       </c>
-      <c r="B38" s="8" t="inlineStr">
-        <is>
-          <t>UNCATEGORIZED</t>
-        </is>
-      </c>
-      <c r="C38" s="8" t="inlineStr">
+      <c r="B39" s="8" t="inlineStr">
+        <is>
+          <t>UNCATEGORIZED</t>
+        </is>
+      </c>
+      <c r="C39" s="8" t="inlineStr">
         <is>
           <t>/v2_1_1.1/payments/v2_1_1.1/getPayment.post.parameters</t>
         </is>
       </c>
-      <c r="D38" s="8" t="inlineStr">
+      <c r="D39" s="8" t="inlineStr">
         <is>
           <t xml:space="preserve">- $ref: '#/parameters/authorizationParam'
 - $ref: '#/parameters/acceptEncodingParam'
@@ -1990,7 +2021,7 @@
 </t>
         </is>
       </c>
-      <c r="E38" s="8" t="inlineStr">
+      <c r="E39" s="8" t="inlineStr">
         <is>
           <t xml:space="preserve">- $ref: '#/parameters/authorizationParam'
 - $ref: '#/parameters/acceptEncodingParam'
@@ -2008,30 +2039,30 @@
 </t>
         </is>
       </c>
-      <c r="F38" s="8" t="inlineStr">
+      <c r="F39" s="8" t="inlineStr">
         <is>
           <t>Added:
 • $ref: #/parameters/contentTypeParam</t>
         </is>
       </c>
     </row>
-    <row r="39" ht="60" customHeight="1">
-      <c r="A39" s="7" t="inlineStr">
+    <row r="40" ht="60" customHeight="1">
+      <c r="A40" s="7" t="inlineStr">
         <is>
           <t>PIS</t>
         </is>
       </c>
-      <c r="B39" s="8" t="inlineStr">
-        <is>
-          <t>UNCATEGORIZED</t>
-        </is>
-      </c>
-      <c r="C39" s="8" t="inlineStr">
+      <c r="B40" s="8" t="inlineStr">
+        <is>
+          <t>UNCATEGORIZED</t>
+        </is>
+      </c>
+      <c r="C40" s="8" t="inlineStr">
         <is>
           <t>/v2_1_1.1/payments/v2_1_1.1/getPayment.post.responses.500</t>
         </is>
       </c>
-      <c r="D39" s="8" t="inlineStr">
+      <c r="D40" s="8" t="inlineStr">
         <is>
           <t xml:space="preserve">description: Internal Server Error
 schema:
@@ -2039,8 +2070,8 @@
 </t>
         </is>
       </c>
-      <c r="E39" s="8" t="inlineStr"/>
-      <c r="F39" s="8" t="inlineStr">
+      <c r="E40" s="8" t="inlineStr"/>
+      <c r="F40" s="8" t="inlineStr">
         <is>
           <t>Removed:
 • description: Internal Server Error
@@ -2049,23 +2080,23 @@
         </is>
       </c>
     </row>
-    <row r="40" ht="60" customHeight="1">
-      <c r="A40" s="7" t="inlineStr">
+    <row r="41" ht="60" customHeight="1">
+      <c r="A41" s="7" t="inlineStr">
         <is>
           <t>PIS</t>
         </is>
       </c>
-      <c r="B40" s="8" t="inlineStr">
-        <is>
-          <t>UNCATEGORIZED</t>
-        </is>
-      </c>
-      <c r="C40" s="8" t="inlineStr">
+      <c r="B41" s="8" t="inlineStr">
+        <is>
+          <t>UNCATEGORIZED</t>
+        </is>
+      </c>
+      <c r="C41" s="8" t="inlineStr">
         <is>
           <t>/v2_1_1.1/payments/v2_1_1.1/getPayment.post.responses.503</t>
         </is>
       </c>
-      <c r="D40" s="8" t="inlineStr">
+      <c r="D41" s="8" t="inlineStr">
         <is>
           <t xml:space="preserve">description: Service Unavailable
 schema:
@@ -2073,8 +2104,8 @@
 </t>
         </is>
       </c>
-      <c r="E40" s="8" t="inlineStr"/>
-      <c r="F40" s="8" t="inlineStr">
+      <c r="E41" s="8" t="inlineStr"/>
+      <c r="F41" s="8" t="inlineStr">
         <is>
           <t>Removed:
 • description: Service Unavailable
@@ -2083,24 +2114,24 @@
         </is>
       </c>
     </row>
-    <row r="41" ht="60" customHeight="1">
-      <c r="A41" s="7" t="inlineStr">
+    <row r="42" ht="60" customHeight="1">
+      <c r="A42" s="7" t="inlineStr">
         <is>
           <t>PIS</t>
         </is>
       </c>
-      <c r="B41" s="8" t="inlineStr">
-        <is>
-          <t>UNCATEGORIZED</t>
-        </is>
-      </c>
-      <c r="C41" s="8" t="inlineStr">
+      <c r="B42" s="8" t="inlineStr">
+        <is>
+          <t>UNCATEGORIZED</t>
+        </is>
+      </c>
+      <c r="C42" s="8" t="inlineStr">
         <is>
           <t>/v2_1_1.1/payments/v2_1_1.1/getPayment.post.responses.510</t>
         </is>
       </c>
-      <c r="D41" s="8" t="inlineStr"/>
-      <c r="E41" s="8" t="inlineStr">
+      <c r="D42" s="8" t="inlineStr"/>
+      <c r="E42" s="8" t="inlineStr">
         <is>
           <t xml:space="preserve">description: Internal Server Error
 schema:
@@ -2108,7 +2139,7 @@
 </t>
         </is>
       </c>
-      <c r="F41" s="8" t="inlineStr">
+      <c r="F42" s="8" t="inlineStr">
         <is>
           <t>Added:
 • description: Internal Server Error
@@ -2117,23 +2148,23 @@
         </is>
       </c>
     </row>
-    <row r="42" ht="75" customHeight="1">
-      <c r="A42" s="7" t="inlineStr">
+    <row r="43" ht="75" customHeight="1">
+      <c r="A43" s="7" t="inlineStr">
         <is>
           <t>PIS</t>
         </is>
       </c>
-      <c r="B42" s="8" t="inlineStr">
-        <is>
-          <t>UNCATEGORIZED</t>
-        </is>
-      </c>
-      <c r="C42" s="8" t="inlineStr">
+      <c r="B43" s="8" t="inlineStr">
+        <is>
+          <t>UNCATEGORIZED</t>
+        </is>
+      </c>
+      <c r="C43" s="8" t="inlineStr">
         <is>
           <t>/v2_1_1.1/payments/v2_1_1.1/getPayment.post.security</t>
         </is>
       </c>
-      <c r="D42" s="8" t="inlineStr">
+      <c r="D43" s="8" t="inlineStr">
         <is>
           <t xml:space="preserve">- xs2a_auth_aspsp:
   - pis
@@ -2142,14 +2173,14 @@
 </t>
         </is>
       </c>
-      <c r="E42" s="8" t="inlineStr">
+      <c r="E43" s="8" t="inlineStr">
         <is>
           <t xml:space="preserve">- xs2a_auth_decoupled:
   - pis
 </t>
         </is>
       </c>
-      <c r="F42" s="8" t="inlineStr">
+      <c r="F43" s="8" t="inlineStr">
         <is>
           <t>Removed:
 • xs2a_auth_aspsp:
@@ -2157,54 +2188,54 @@
         </is>
       </c>
     </row>
-    <row r="43" ht="45" customHeight="1">
-      <c r="A43" s="7" t="inlineStr">
+    <row r="44" ht="45" customHeight="1">
+      <c r="A44" s="7" t="inlineStr">
         <is>
           <t>PIS</t>
         </is>
       </c>
-      <c r="B43" s="8" t="inlineStr">
-        <is>
-          <t>UNCATEGORIZED</t>
-        </is>
-      </c>
-      <c r="C43" s="8" t="inlineStr">
+      <c r="B44" s="8" t="inlineStr">
+        <is>
+          <t>UNCATEGORIZED</t>
+        </is>
+      </c>
+      <c r="C44" s="8" t="inlineStr">
         <is>
           <t>/v2_1_1.1/payments/v2_1_1.1/getBundle.x-swagger-router-controller</t>
         </is>
       </c>
-      <c r="D43" s="8" t="inlineStr">
+      <c r="D44" s="8" t="inlineStr">
         <is>
           <t xml:space="preserve">pis
 ...
 </t>
         </is>
       </c>
-      <c r="E43" s="8" t="inlineStr"/>
-      <c r="F43" s="8" t="inlineStr">
+      <c r="E44" s="8" t="inlineStr"/>
+      <c r="F44" s="8" t="inlineStr">
         <is>
           <t>Removed:
 • pis</t>
         </is>
       </c>
     </row>
-    <row r="44" ht="210" customHeight="1">
-      <c r="A44" s="7" t="inlineStr">
+    <row r="45" ht="210" customHeight="1">
+      <c r="A45" s="7" t="inlineStr">
         <is>
           <t>PIS</t>
         </is>
       </c>
-      <c r="B44" s="8" t="inlineStr">
-        <is>
-          <t>UNCATEGORIZED</t>
-        </is>
-      </c>
-      <c r="C44" s="8" t="inlineStr">
+      <c r="B45" s="8" t="inlineStr">
+        <is>
+          <t>UNCATEGORIZED</t>
+        </is>
+      </c>
+      <c r="C45" s="8" t="inlineStr">
         <is>
           <t>/v2_1_1.1/payments/v2_1_1.1/getBundle.post.parameters</t>
         </is>
       </c>
-      <c r="D44" s="8" t="inlineStr">
+      <c r="D45" s="8" t="inlineStr">
         <is>
           <t xml:space="preserve">- $ref: '#/parameters/authorizationParam'
 - $ref: '#/parameters/acceptEncodingParam'
@@ -2221,7 +2252,7 @@
 </t>
         </is>
       </c>
-      <c r="E44" s="8" t="inlineStr">
+      <c r="E45" s="8" t="inlineStr">
         <is>
           <t xml:space="preserve">- $ref: '#/parameters/authorizationParam'
 - $ref: '#/parameters/acceptEncodingParam'
@@ -2239,30 +2270,30 @@
 </t>
         </is>
       </c>
-      <c r="F44" s="8" t="inlineStr">
+      <c r="F45" s="8" t="inlineStr">
         <is>
           <t>Added:
 • $ref: #/parameters/contentTypeParam</t>
         </is>
       </c>
     </row>
-    <row r="45" ht="60" customHeight="1">
-      <c r="A45" s="7" t="inlineStr">
+    <row r="46" ht="60" customHeight="1">
+      <c r="A46" s="7" t="inlineStr">
         <is>
           <t>PIS</t>
         </is>
       </c>
-      <c r="B45" s="8" t="inlineStr">
-        <is>
-          <t>UNCATEGORIZED</t>
-        </is>
-      </c>
-      <c r="C45" s="8" t="inlineStr">
+      <c r="B46" s="8" t="inlineStr">
+        <is>
+          <t>UNCATEGORIZED</t>
+        </is>
+      </c>
+      <c r="C46" s="8" t="inlineStr">
         <is>
           <t>/v2_1_1.1/payments/v2_1_1.1/getBundle.post.responses.500</t>
         </is>
       </c>
-      <c r="D45" s="8" t="inlineStr">
+      <c r="D46" s="8" t="inlineStr">
         <is>
           <t xml:space="preserve">description: Internal Server Error
 schema:
@@ -2270,8 +2301,8 @@
 </t>
         </is>
       </c>
-      <c r="E45" s="8" t="inlineStr"/>
-      <c r="F45" s="8" t="inlineStr">
+      <c r="E46" s="8" t="inlineStr"/>
+      <c r="F46" s="8" t="inlineStr">
         <is>
           <t>Removed:
 • description: Internal Server Error
@@ -2280,23 +2311,23 @@
         </is>
       </c>
     </row>
-    <row r="46" ht="60" customHeight="1">
-      <c r="A46" s="7" t="inlineStr">
+    <row r="47" ht="60" customHeight="1">
+      <c r="A47" s="7" t="inlineStr">
         <is>
           <t>PIS</t>
         </is>
       </c>
-      <c r="B46" s="8" t="inlineStr">
-        <is>
-          <t>UNCATEGORIZED</t>
-        </is>
-      </c>
-      <c r="C46" s="8" t="inlineStr">
+      <c r="B47" s="8" t="inlineStr">
+        <is>
+          <t>UNCATEGORIZED</t>
+        </is>
+      </c>
+      <c r="C47" s="8" t="inlineStr">
         <is>
           <t>/v2_1_1.1/payments/v2_1_1.1/getBundle.post.responses.503</t>
         </is>
       </c>
-      <c r="D46" s="8" t="inlineStr">
+      <c r="D47" s="8" t="inlineStr">
         <is>
           <t xml:space="preserve">description: Service Unavailable
 schema:
@@ -2304,8 +2335,8 @@
 </t>
         </is>
       </c>
-      <c r="E46" s="8" t="inlineStr"/>
-      <c r="F46" s="8" t="inlineStr">
+      <c r="E47" s="8" t="inlineStr"/>
+      <c r="F47" s="8" t="inlineStr">
         <is>
           <t>Removed:
 • description: Service Unavailable
@@ -2314,24 +2345,24 @@
         </is>
       </c>
     </row>
-    <row r="47" ht="60" customHeight="1">
-      <c r="A47" s="7" t="inlineStr">
+    <row r="48" ht="60" customHeight="1">
+      <c r="A48" s="7" t="inlineStr">
         <is>
           <t>PIS</t>
         </is>
       </c>
-      <c r="B47" s="8" t="inlineStr">
-        <is>
-          <t>UNCATEGORIZED</t>
-        </is>
-      </c>
-      <c r="C47" s="8" t="inlineStr">
+      <c r="B48" s="8" t="inlineStr">
+        <is>
+          <t>UNCATEGORIZED</t>
+        </is>
+      </c>
+      <c r="C48" s="8" t="inlineStr">
         <is>
           <t>/v2_1_1.1/payments/v2_1_1.1/getBundle.post.responses.510</t>
         </is>
       </c>
-      <c r="D47" s="8" t="inlineStr"/>
-      <c r="E47" s="8" t="inlineStr">
+      <c r="D48" s="8" t="inlineStr"/>
+      <c r="E48" s="8" t="inlineStr">
         <is>
           <t xml:space="preserve">description: Internal Server Error
 schema:
@@ -2339,7 +2370,7 @@
 </t>
         </is>
       </c>
-      <c r="F47" s="8" t="inlineStr">
+      <c r="F48" s="8" t="inlineStr">
         <is>
           <t>Added:
 • description: Internal Server Error
@@ -2348,23 +2379,23 @@
         </is>
       </c>
     </row>
-    <row r="48" ht="75" customHeight="1">
-      <c r="A48" s="7" t="inlineStr">
+    <row r="49" ht="75" customHeight="1">
+      <c r="A49" s="7" t="inlineStr">
         <is>
           <t>PIS</t>
         </is>
       </c>
-      <c r="B48" s="8" t="inlineStr">
-        <is>
-          <t>UNCATEGORIZED</t>
-        </is>
-      </c>
-      <c r="C48" s="8" t="inlineStr">
+      <c r="B49" s="8" t="inlineStr">
+        <is>
+          <t>UNCATEGORIZED</t>
+        </is>
+      </c>
+      <c r="C49" s="8" t="inlineStr">
         <is>
           <t>/v2_1_1.1/payments/v2_1_1.1/getBundle.post.security</t>
         </is>
       </c>
-      <c r="D48" s="8" t="inlineStr">
+      <c r="D49" s="8" t="inlineStr">
         <is>
           <t xml:space="preserve">- xs2a_auth_aspsp:
   - pis
@@ -2373,14 +2404,14 @@
 </t>
         </is>
       </c>
-      <c r="E48" s="8" t="inlineStr">
+      <c r="E49" s="8" t="inlineStr">
         <is>
           <t xml:space="preserve">- xs2a_auth_decoupled:
   - pis
 </t>
         </is>
       </c>
-      <c r="F48" s="8" t="inlineStr">
+      <c r="F49" s="8" t="inlineStr">
         <is>
           <t>Removed:
 • xs2a_auth_aspsp:
@@ -2388,54 +2419,54 @@
         </is>
       </c>
     </row>
-    <row r="49" ht="45" customHeight="1">
-      <c r="A49" s="7" t="inlineStr">
+    <row r="50" ht="45" customHeight="1">
+      <c r="A50" s="7" t="inlineStr">
         <is>
           <t>PIS</t>
         </is>
       </c>
-      <c r="B49" s="8" t="inlineStr">
-        <is>
-          <t>UNCATEGORIZED</t>
-        </is>
-      </c>
-      <c r="C49" s="8" t="inlineStr">
+      <c r="B50" s="8" t="inlineStr">
+        <is>
+          <t>UNCATEGORIZED</t>
+        </is>
+      </c>
+      <c r="C50" s="8" t="inlineStr">
         <is>
           <t>/v2_1_1.1/payments/v2_1_1.1/getRecurringPayment.x-swagger-router-controller</t>
         </is>
       </c>
-      <c r="D49" s="8" t="inlineStr">
+      <c r="D50" s="8" t="inlineStr">
         <is>
           <t xml:space="preserve">pis
 ...
 </t>
         </is>
       </c>
-      <c r="E49" s="8" t="inlineStr"/>
-      <c r="F49" s="8" t="inlineStr">
+      <c r="E50" s="8" t="inlineStr"/>
+      <c r="F50" s="8" t="inlineStr">
         <is>
           <t>Removed:
 • pis</t>
         </is>
       </c>
     </row>
-    <row r="50" ht="210" customHeight="1">
-      <c r="A50" s="7" t="inlineStr">
+    <row r="51" ht="210" customHeight="1">
+      <c r="A51" s="7" t="inlineStr">
         <is>
           <t>PIS</t>
         </is>
       </c>
-      <c r="B50" s="8" t="inlineStr">
-        <is>
-          <t>UNCATEGORIZED</t>
-        </is>
-      </c>
-      <c r="C50" s="8" t="inlineStr">
+      <c r="B51" s="8" t="inlineStr">
+        <is>
+          <t>UNCATEGORIZED</t>
+        </is>
+      </c>
+      <c r="C51" s="8" t="inlineStr">
         <is>
           <t>/v2_1_1.1/payments/v2_1_1.1/getRecurringPayment.post.parameters</t>
         </is>
       </c>
-      <c r="D50" s="8" t="inlineStr">
+      <c r="D51" s="8" t="inlineStr">
         <is>
           <t xml:space="preserve">- $ref: '#/parameters/authorizationParam'
 - $ref: '#/parameters/acceptEncodingParam'
@@ -2452,7 +2483,7 @@
 </t>
         </is>
       </c>
-      <c r="E50" s="8" t="inlineStr">
+      <c r="E51" s="8" t="inlineStr">
         <is>
           <t xml:space="preserve">- $ref: '#/parameters/authorizationParam'
 - $ref: '#/parameters/acceptEncodingParam'
@@ -2470,30 +2501,30 @@
 </t>
         </is>
       </c>
-      <c r="F50" s="8" t="inlineStr">
+      <c r="F51" s="8" t="inlineStr">
         <is>
           <t>Added:
 • $ref: #/parameters/contentTypeParam</t>
         </is>
       </c>
     </row>
-    <row r="51" ht="60" customHeight="1">
-      <c r="A51" s="7" t="inlineStr">
+    <row r="52" ht="60" customHeight="1">
+      <c r="A52" s="7" t="inlineStr">
         <is>
           <t>PIS</t>
         </is>
       </c>
-      <c r="B51" s="8" t="inlineStr">
-        <is>
-          <t>UNCATEGORIZED</t>
-        </is>
-      </c>
-      <c r="C51" s="8" t="inlineStr">
+      <c r="B52" s="8" t="inlineStr">
+        <is>
+          <t>UNCATEGORIZED</t>
+        </is>
+      </c>
+      <c r="C52" s="8" t="inlineStr">
         <is>
           <t>/v2_1_1.1/payments/v2_1_1.1/getRecurringPayment.post.responses.500</t>
         </is>
       </c>
-      <c r="D51" s="8" t="inlineStr">
+      <c r="D52" s="8" t="inlineStr">
         <is>
           <t xml:space="preserve">description: Internal Server Error
 schema:
@@ -2501,8 +2532,8 @@
 </t>
         </is>
       </c>
-      <c r="E51" s="8" t="inlineStr"/>
-      <c r="F51" s="8" t="inlineStr">
+      <c r="E52" s="8" t="inlineStr"/>
+      <c r="F52" s="8" t="inlineStr">
         <is>
           <t>Removed:
 • description: Internal Server Error
@@ -2511,23 +2542,23 @@
         </is>
       </c>
     </row>
-    <row r="52" ht="60" customHeight="1">
-      <c r="A52" s="7" t="inlineStr">
+    <row r="53" ht="60" customHeight="1">
+      <c r="A53" s="7" t="inlineStr">
         <is>
           <t>PIS</t>
         </is>
       </c>
-      <c r="B52" s="8" t="inlineStr">
-        <is>
-          <t>UNCATEGORIZED</t>
-        </is>
-      </c>
-      <c r="C52" s="8" t="inlineStr">
+      <c r="B53" s="8" t="inlineStr">
+        <is>
+          <t>UNCATEGORIZED</t>
+        </is>
+      </c>
+      <c r="C53" s="8" t="inlineStr">
         <is>
           <t>/v2_1_1.1/payments/v2_1_1.1/getRecurringPayment.post.responses.503</t>
         </is>
       </c>
-      <c r="D52" s="8" t="inlineStr">
+      <c r="D53" s="8" t="inlineStr">
         <is>
           <t xml:space="preserve">description: Service Unavailable
 schema:
@@ -2535,8 +2566,8 @@
 </t>
         </is>
       </c>
-      <c r="E52" s="8" t="inlineStr"/>
-      <c r="F52" s="8" t="inlineStr">
+      <c r="E53" s="8" t="inlineStr"/>
+      <c r="F53" s="8" t="inlineStr">
         <is>
           <t>Removed:
 • description: Service Unavailable
@@ -2545,24 +2576,24 @@
         </is>
       </c>
     </row>
-    <row r="53" ht="60" customHeight="1">
-      <c r="A53" s="7" t="inlineStr">
+    <row r="54" ht="60" customHeight="1">
+      <c r="A54" s="7" t="inlineStr">
         <is>
           <t>PIS</t>
         </is>
       </c>
-      <c r="B53" s="8" t="inlineStr">
-        <is>
-          <t>UNCATEGORIZED</t>
-        </is>
-      </c>
-      <c r="C53" s="8" t="inlineStr">
+      <c r="B54" s="8" t="inlineStr">
+        <is>
+          <t>UNCATEGORIZED</t>
+        </is>
+      </c>
+      <c r="C54" s="8" t="inlineStr">
         <is>
           <t>/v2_1_1.1/payments/v2_1_1.1/getRecurringPayment.post.responses.510</t>
         </is>
       </c>
-      <c r="D53" s="8" t="inlineStr"/>
-      <c r="E53" s="8" t="inlineStr">
+      <c r="D54" s="8" t="inlineStr"/>
+      <c r="E54" s="8" t="inlineStr">
         <is>
           <t xml:space="preserve">description: Internal Server Error
 schema:
@@ -2570,7 +2601,7 @@
 </t>
         </is>
       </c>
-      <c r="F53" s="8" t="inlineStr">
+      <c r="F54" s="8" t="inlineStr">
         <is>
           <t>Added:
 • description: Internal Server Error
@@ -2579,23 +2610,23 @@
         </is>
       </c>
     </row>
-    <row r="54" ht="75" customHeight="1">
-      <c r="A54" s="7" t="inlineStr">
+    <row r="55" ht="75" customHeight="1">
+      <c r="A55" s="7" t="inlineStr">
         <is>
           <t>PIS</t>
         </is>
       </c>
-      <c r="B54" s="8" t="inlineStr">
-        <is>
-          <t>UNCATEGORIZED</t>
-        </is>
-      </c>
-      <c r="C54" s="8" t="inlineStr">
+      <c r="B55" s="8" t="inlineStr">
+        <is>
+          <t>UNCATEGORIZED</t>
+        </is>
+      </c>
+      <c r="C55" s="8" t="inlineStr">
         <is>
           <t>/v2_1_1.1/payments/v2_1_1.1/getRecurringPayment.post.security</t>
         </is>
       </c>
-      <c r="D54" s="8" t="inlineStr">
+      <c r="D55" s="8" t="inlineStr">
         <is>
           <t xml:space="preserve">- xs2a_auth_aspsp:
   - pis
@@ -2604,14 +2635,14 @@
 </t>
         </is>
       </c>
-      <c r="E54" s="8" t="inlineStr">
+      <c r="E55" s="8" t="inlineStr">
         <is>
           <t xml:space="preserve">- xs2a_auth_decoupled:
   - pis
 </t>
         </is>
       </c>
-      <c r="F54" s="8" t="inlineStr">
+      <c r="F55" s="8" t="inlineStr">
         <is>
           <t>Removed:
 • xs2a_auth_aspsp:
@@ -2619,23 +2650,23 @@
         </is>
       </c>
     </row>
-    <row r="55" ht="1020" customHeight="1">
-      <c r="A55" s="7" t="inlineStr">
+    <row r="56" ht="1020" customHeight="1">
+      <c r="A56" s="7" t="inlineStr">
         <is>
           <t>PIS</t>
         </is>
       </c>
-      <c r="B55" s="8" t="inlineStr">
-        <is>
-          <t>UNCATEGORIZED</t>
-        </is>
-      </c>
-      <c r="C55" s="8" t="inlineStr">
+      <c r="B56" s="8" t="inlineStr">
+        <is>
+          <t>UNCATEGORIZED</t>
+        </is>
+      </c>
+      <c r="C56" s="8" t="inlineStr">
         <is>
           <t>/v2_1_1.1/payments/v2_1_1.1/getMultiplePayments</t>
         </is>
       </c>
-      <c r="D55" s="8" t="inlineStr">
+      <c r="D56" s="8" t="inlineStr">
         <is>
           <t xml:space="preserve">x-swagger-router-controller: pis
 post:
@@ -2707,8 +2738,8 @@
 </t>
         </is>
       </c>
-      <c r="E55" s="8" t="inlineStr"/>
-      <c r="F55" s="8" t="inlineStr">
+      <c r="E56" s="8" t="inlineStr"/>
+      <c r="F56" s="8" t="inlineStr">
         <is>
           <t>Removed:
 • x-swagger-router-controller: pis
@@ -2781,54 +2812,54 @@
         </is>
       </c>
     </row>
-    <row r="56" ht="45" customHeight="1">
-      <c r="A56" s="7" t="inlineStr">
+    <row r="57" ht="45" customHeight="1">
+      <c r="A57" s="7" t="inlineStr">
         <is>
           <t>PIS</t>
         </is>
       </c>
-      <c r="B56" s="8" t="inlineStr">
-        <is>
-          <t>UNCATEGORIZED</t>
-        </is>
-      </c>
-      <c r="C56" s="8" t="inlineStr">
+      <c r="B57" s="8" t="inlineStr">
+        <is>
+          <t>UNCATEGORIZED</t>
+        </is>
+      </c>
+      <c r="C57" s="8" t="inlineStr">
         <is>
           <t>/v2_1_1.1/payments/v2_1_1.1/cancelPayments.x-swagger-router-controller</t>
         </is>
       </c>
-      <c r="D56" s="8" t="inlineStr">
+      <c r="D57" s="8" t="inlineStr">
         <is>
           <t xml:space="preserve">pis
 ...
 </t>
         </is>
       </c>
-      <c r="E56" s="8" t="inlineStr"/>
-      <c r="F56" s="8" t="inlineStr">
+      <c r="E57" s="8" t="inlineStr"/>
+      <c r="F57" s="8" t="inlineStr">
         <is>
           <t>Removed:
 • pis</t>
         </is>
       </c>
     </row>
-    <row r="57" ht="210" customHeight="1">
-      <c r="A57" s="7" t="inlineStr">
+    <row r="58" ht="210" customHeight="1">
+      <c r="A58" s="7" t="inlineStr">
         <is>
           <t>PIS</t>
         </is>
       </c>
-      <c r="B57" s="8" t="inlineStr">
-        <is>
-          <t>UNCATEGORIZED</t>
-        </is>
-      </c>
-      <c r="C57" s="8" t="inlineStr">
+      <c r="B58" s="8" t="inlineStr">
+        <is>
+          <t>UNCATEGORIZED</t>
+        </is>
+      </c>
+      <c r="C58" s="8" t="inlineStr">
         <is>
           <t>/v2_1_1.1/payments/v2_1_1.1/cancelPayments.post.parameters</t>
         </is>
       </c>
-      <c r="D57" s="8" t="inlineStr">
+      <c r="D58" s="8" t="inlineStr">
         <is>
           <t xml:space="preserve">- $ref: '#/parameters/authorizationParam'
 - $ref: '#/parameters/acceptEncodingParam'
@@ -2845,7 +2876,7 @@
 </t>
         </is>
       </c>
-      <c r="E57" s="8" t="inlineStr">
+      <c r="E58" s="8" t="inlineStr">
         <is>
           <t xml:space="preserve">- $ref: '#/parameters/authorizationParam'
 - $ref: '#/parameters/acceptEncodingParam'
@@ -2863,30 +2894,30 @@
 </t>
         </is>
       </c>
-      <c r="F57" s="8" t="inlineStr">
+      <c r="F58" s="8" t="inlineStr">
         <is>
           <t>Added:
 • $ref: #/parameters/contentTypeParam</t>
         </is>
       </c>
     </row>
-    <row r="58" ht="60" customHeight="1">
-      <c r="A58" s="7" t="inlineStr">
+    <row r="59" ht="60" customHeight="1">
+      <c r="A59" s="7" t="inlineStr">
         <is>
           <t>PIS</t>
         </is>
       </c>
-      <c r="B58" s="8" t="inlineStr">
-        <is>
-          <t>UNCATEGORIZED</t>
-        </is>
-      </c>
-      <c r="C58" s="8" t="inlineStr">
+      <c r="B59" s="8" t="inlineStr">
+        <is>
+          <t>UNCATEGORIZED</t>
+        </is>
+      </c>
+      <c r="C59" s="8" t="inlineStr">
         <is>
           <t>/v2_1_1.1/payments/v2_1_1.1/cancelPayments.post.responses.500</t>
         </is>
       </c>
-      <c r="D58" s="8" t="inlineStr">
+      <c r="D59" s="8" t="inlineStr">
         <is>
           <t xml:space="preserve">description: Internal Server Error
 schema:
@@ -2894,8 +2925,8 @@
 </t>
         </is>
       </c>
-      <c r="E58" s="8" t="inlineStr"/>
-      <c r="F58" s="8" t="inlineStr">
+      <c r="E59" s="8" t="inlineStr"/>
+      <c r="F59" s="8" t="inlineStr">
         <is>
           <t>Removed:
 • description: Internal Server Error
@@ -2904,23 +2935,23 @@
         </is>
       </c>
     </row>
-    <row r="59" ht="60" customHeight="1">
-      <c r="A59" s="7" t="inlineStr">
+    <row r="60" ht="60" customHeight="1">
+      <c r="A60" s="7" t="inlineStr">
         <is>
           <t>PIS</t>
         </is>
       </c>
-      <c r="B59" s="8" t="inlineStr">
-        <is>
-          <t>UNCATEGORIZED</t>
-        </is>
-      </c>
-      <c r="C59" s="8" t="inlineStr">
+      <c r="B60" s="8" t="inlineStr">
+        <is>
+          <t>UNCATEGORIZED</t>
+        </is>
+      </c>
+      <c r="C60" s="8" t="inlineStr">
         <is>
           <t>/v2_1_1.1/payments/v2_1_1.1/cancelPayments.post.responses.503</t>
         </is>
       </c>
-      <c r="D59" s="8" t="inlineStr">
+      <c r="D60" s="8" t="inlineStr">
         <is>
           <t xml:space="preserve">description: Service Unavailable
 schema:
@@ -2928,8 +2959,8 @@
 </t>
         </is>
       </c>
-      <c r="E59" s="8" t="inlineStr"/>
-      <c r="F59" s="8" t="inlineStr">
+      <c r="E60" s="8" t="inlineStr"/>
+      <c r="F60" s="8" t="inlineStr">
         <is>
           <t>Removed:
 • description: Service Unavailable
@@ -2938,24 +2969,24 @@
         </is>
       </c>
     </row>
-    <row r="60" ht="60" customHeight="1">
-      <c r="A60" s="7" t="inlineStr">
+    <row r="61" ht="60" customHeight="1">
+      <c r="A61" s="7" t="inlineStr">
         <is>
           <t>PIS</t>
         </is>
       </c>
-      <c r="B60" s="8" t="inlineStr">
-        <is>
-          <t>UNCATEGORIZED</t>
-        </is>
-      </c>
-      <c r="C60" s="8" t="inlineStr">
+      <c r="B61" s="8" t="inlineStr">
+        <is>
+          <t>UNCATEGORIZED</t>
+        </is>
+      </c>
+      <c r="C61" s="8" t="inlineStr">
         <is>
           <t>/v2_1_1.1/payments/v2_1_1.1/cancelPayments.post.responses.510</t>
         </is>
       </c>
-      <c r="D60" s="8" t="inlineStr"/>
-      <c r="E60" s="8" t="inlineStr">
+      <c r="D61" s="8" t="inlineStr"/>
+      <c r="E61" s="8" t="inlineStr">
         <is>
           <t xml:space="preserve">description: Internal Server Error
 schema:
@@ -2963,7 +2994,7 @@
 </t>
         </is>
       </c>
-      <c r="F60" s="8" t="inlineStr">
+      <c r="F61" s="8" t="inlineStr">
         <is>
           <t>Added:
 • description: Internal Server Error
@@ -2972,23 +3003,23 @@
         </is>
       </c>
     </row>
-    <row r="61" ht="75" customHeight="1">
-      <c r="A61" s="7" t="inlineStr">
+    <row r="62" ht="75" customHeight="1">
+      <c r="A62" s="7" t="inlineStr">
         <is>
           <t>PIS</t>
         </is>
       </c>
-      <c r="B61" s="8" t="inlineStr">
-        <is>
-          <t>UNCATEGORIZED</t>
-        </is>
-      </c>
-      <c r="C61" s="8" t="inlineStr">
+      <c r="B62" s="8" t="inlineStr">
+        <is>
+          <t>UNCATEGORIZED</t>
+        </is>
+      </c>
+      <c r="C62" s="8" t="inlineStr">
         <is>
           <t>/v2_1_1.1/payments/v2_1_1.1/cancelPayments.post.security</t>
         </is>
       </c>
-      <c r="D61" s="8" t="inlineStr">
+      <c r="D62" s="8" t="inlineStr">
         <is>
           <t xml:space="preserve">- xs2a_auth_aspsp:
   - pis
@@ -2997,14 +3028,14 @@
 </t>
         </is>
       </c>
-      <c r="E61" s="8" t="inlineStr">
+      <c r="E62" s="8" t="inlineStr">
         <is>
           <t xml:space="preserve">- xs2a_auth_decoupled:
   - pis
 </t>
         </is>
       </c>
-      <c r="F61" s="8" t="inlineStr">
+      <c r="F62" s="8" t="inlineStr">
         <is>
           <t>Removed:
 • xs2a_auth_aspsp:
@@ -3012,54 +3043,54 @@
         </is>
       </c>
     </row>
-    <row r="62" ht="45" customHeight="1">
-      <c r="A62" s="7" t="inlineStr">
+    <row r="63" ht="45" customHeight="1">
+      <c r="A63" s="7" t="inlineStr">
         <is>
           <t>PIS</t>
         </is>
       </c>
-      <c r="B62" s="8" t="inlineStr">
-        <is>
-          <t>UNCATEGORIZED</t>
-        </is>
-      </c>
-      <c r="C62" s="8" t="inlineStr">
+      <c r="B63" s="8" t="inlineStr">
+        <is>
+          <t>UNCATEGORIZED</t>
+        </is>
+      </c>
+      <c r="C63" s="8" t="inlineStr">
         <is>
           <t>/v2_1_1.1/payments/v2_1_1.1/cancelRecurringPayment.x-swagger-router-controller</t>
         </is>
       </c>
-      <c r="D62" s="8" t="inlineStr">
+      <c r="D63" s="8" t="inlineStr">
         <is>
           <t xml:space="preserve">pis
 ...
 </t>
         </is>
       </c>
-      <c r="E62" s="8" t="inlineStr"/>
-      <c r="F62" s="8" t="inlineStr">
+      <c r="E63" s="8" t="inlineStr"/>
+      <c r="F63" s="8" t="inlineStr">
         <is>
           <t>Removed:
 • pis</t>
         </is>
       </c>
     </row>
-    <row r="63" ht="210" customHeight="1">
-      <c r="A63" s="7" t="inlineStr">
+    <row r="64" ht="210" customHeight="1">
+      <c r="A64" s="7" t="inlineStr">
         <is>
           <t>PIS</t>
         </is>
       </c>
-      <c r="B63" s="8" t="inlineStr">
-        <is>
-          <t>UNCATEGORIZED</t>
-        </is>
-      </c>
-      <c r="C63" s="8" t="inlineStr">
+      <c r="B64" s="8" t="inlineStr">
+        <is>
+          <t>UNCATEGORIZED</t>
+        </is>
+      </c>
+      <c r="C64" s="8" t="inlineStr">
         <is>
           <t>/v2_1_1.1/payments/v2_1_1.1/cancelRecurringPayment.post.parameters</t>
         </is>
       </c>
-      <c r="D63" s="8" t="inlineStr">
+      <c r="D64" s="8" t="inlineStr">
         <is>
           <t xml:space="preserve">- $ref: '#/parameters/authorizationParam'
 - $ref: '#/parameters/acceptEncodingParam'
@@ -3076,7 +3107,7 @@
 </t>
         </is>
       </c>
-      <c r="E63" s="8" t="inlineStr">
+      <c r="E64" s="8" t="inlineStr">
         <is>
           <t xml:space="preserve">- $ref: '#/parameters/authorizationParam'
 - $ref: '#/parameters/acceptEncodingParam'
@@ -3094,30 +3125,30 @@
 </t>
         </is>
       </c>
-      <c r="F63" s="8" t="inlineStr">
+      <c r="F64" s="8" t="inlineStr">
         <is>
           <t>Added:
 • $ref: #/parameters/contentTypeParam</t>
         </is>
       </c>
     </row>
-    <row r="64" ht="60" customHeight="1">
-      <c r="A64" s="7" t="inlineStr">
+    <row r="65" ht="60" customHeight="1">
+      <c r="A65" s="7" t="inlineStr">
         <is>
           <t>PIS</t>
         </is>
       </c>
-      <c r="B64" s="8" t="inlineStr">
-        <is>
-          <t>UNCATEGORIZED</t>
-        </is>
-      </c>
-      <c r="C64" s="8" t="inlineStr">
+      <c r="B65" s="8" t="inlineStr">
+        <is>
+          <t>UNCATEGORIZED</t>
+        </is>
+      </c>
+      <c r="C65" s="8" t="inlineStr">
         <is>
           <t>/v2_1_1.1/payments/v2_1_1.1/cancelRecurringPayment.post.responses.500</t>
         </is>
       </c>
-      <c r="D64" s="8" t="inlineStr">
+      <c r="D65" s="8" t="inlineStr">
         <is>
           <t xml:space="preserve">description: Internal Server Error
 schema:
@@ -3125,8 +3156,8 @@
 </t>
         </is>
       </c>
-      <c r="E64" s="8" t="inlineStr"/>
-      <c r="F64" s="8" t="inlineStr">
+      <c r="E65" s="8" t="inlineStr"/>
+      <c r="F65" s="8" t="inlineStr">
         <is>
           <t>Removed:
 • description: Internal Server Error
@@ -3135,23 +3166,23 @@
         </is>
       </c>
     </row>
-    <row r="65" ht="60" customHeight="1">
-      <c r="A65" s="7" t="inlineStr">
+    <row r="66" ht="60" customHeight="1">
+      <c r="A66" s="7" t="inlineStr">
         <is>
           <t>PIS</t>
         </is>
       </c>
-      <c r="B65" s="8" t="inlineStr">
-        <is>
-          <t>UNCATEGORIZED</t>
-        </is>
-      </c>
-      <c r="C65" s="8" t="inlineStr">
+      <c r="B66" s="8" t="inlineStr">
+        <is>
+          <t>UNCATEGORIZED</t>
+        </is>
+      </c>
+      <c r="C66" s="8" t="inlineStr">
         <is>
           <t>/v2_1_1.1/payments/v2_1_1.1/cancelRecurringPayment.post.responses.503</t>
         </is>
       </c>
-      <c r="D65" s="8" t="inlineStr">
+      <c r="D66" s="8" t="inlineStr">
         <is>
           <t xml:space="preserve">description: Service Unavailable
 schema:
@@ -3159,8 +3190,8 @@
 </t>
         </is>
       </c>
-      <c r="E65" s="8" t="inlineStr"/>
-      <c r="F65" s="8" t="inlineStr">
+      <c r="E66" s="8" t="inlineStr"/>
+      <c r="F66" s="8" t="inlineStr">
         <is>
           <t>Removed:
 • description: Service Unavailable
@@ -3169,24 +3200,24 @@
         </is>
       </c>
     </row>
-    <row r="66" ht="60" customHeight="1">
-      <c r="A66" s="7" t="inlineStr">
+    <row r="67" ht="60" customHeight="1">
+      <c r="A67" s="7" t="inlineStr">
         <is>
           <t>PIS</t>
         </is>
       </c>
-      <c r="B66" s="8" t="inlineStr">
-        <is>
-          <t>UNCATEGORIZED</t>
-        </is>
-      </c>
-      <c r="C66" s="8" t="inlineStr">
+      <c r="B67" s="8" t="inlineStr">
+        <is>
+          <t>UNCATEGORIZED</t>
+        </is>
+      </c>
+      <c r="C67" s="8" t="inlineStr">
         <is>
           <t>/v2_1_1.1/payments/v2_1_1.1/cancelRecurringPayment.post.responses.510</t>
         </is>
       </c>
-      <c r="D66" s="8" t="inlineStr"/>
-      <c r="E66" s="8" t="inlineStr">
+      <c r="D67" s="8" t="inlineStr"/>
+      <c r="E67" s="8" t="inlineStr">
         <is>
           <t xml:space="preserve">description: Internal Server Error
 schema:
@@ -3194,7 +3225,7 @@
 </t>
         </is>
       </c>
-      <c r="F66" s="8" t="inlineStr">
+      <c r="F67" s="8" t="inlineStr">
         <is>
           <t>Added:
 • description: Internal Server Error
@@ -3203,23 +3234,23 @@
         </is>
       </c>
     </row>
-    <row r="67" ht="75" customHeight="1">
-      <c r="A67" s="7" t="inlineStr">
+    <row r="68" ht="75" customHeight="1">
+      <c r="A68" s="7" t="inlineStr">
         <is>
           <t>PIS</t>
         </is>
       </c>
-      <c r="B67" s="8" t="inlineStr">
-        <is>
-          <t>UNCATEGORIZED</t>
-        </is>
-      </c>
-      <c r="C67" s="8" t="inlineStr">
+      <c r="B68" s="8" t="inlineStr">
+        <is>
+          <t>UNCATEGORIZED</t>
+        </is>
+      </c>
+      <c r="C68" s="8" t="inlineStr">
         <is>
           <t>/v2_1_1.1/payments/v2_1_1.1/cancelRecurringPayment.post.security</t>
         </is>
       </c>
-      <c r="D67" s="8" t="inlineStr">
+      <c r="D68" s="8" t="inlineStr">
         <is>
           <t xml:space="preserve">- xs2a_auth_aspsp:
   - pis
@@ -3228,49 +3259,18 @@
 </t>
         </is>
       </c>
-      <c r="E67" s="8" t="inlineStr">
+      <c r="E68" s="8" t="inlineStr">
         <is>
           <t xml:space="preserve">- xs2a_auth_decoupled:
   - pis
 </t>
         </is>
       </c>
-      <c r="F67" s="8" t="inlineStr">
+      <c r="F68" s="8" t="inlineStr">
         <is>
           <t>Removed:
 • xs2a_auth_aspsp:
   -     pis</t>
-        </is>
-      </c>
-    </row>
-    <row r="68" ht="45" customHeight="1">
-      <c r="A68" s="9" t="inlineStr">
-        <is>
-          <t>CAF</t>
-        </is>
-      </c>
-      <c r="B68" s="8" t="inlineStr">
-        <is>
-          <t>HIGH</t>
-        </is>
-      </c>
-      <c r="C68" s="8" t="inlineStr">
-        <is>
-          <t>/v2_1_1.1/confirmation/v2_1_1.1/getConfirmationOfFunds.x-swagger-router-controller</t>
-        </is>
-      </c>
-      <c r="D68" s="8" t="inlineStr">
-        <is>
-          <t xml:space="preserve">caf
-...
-</t>
-        </is>
-      </c>
-      <c r="E68" s="8" t="inlineStr"/>
-      <c r="F68" s="8" t="inlineStr">
-        <is>
-          <t>Removed:
-• caf</t>
         </is>
       </c>
     </row>
@@ -3471,7 +3471,7 @@
       </c>
       <c r="B74" s="8" t="inlineStr">
         <is>
-          <t>MINOR</t>
+          <t>UNCATEGORIZED</t>
         </is>
       </c>
       <c r="C74" s="8" t="inlineStr">

</xml_diff>

<commit_message>
Refactor app/routes.py to handle file upload restrictions
</commit_message>
<xml_diff>
--- a/reports/report.xlsx
+++ b/reports/report.xlsx
@@ -579,7 +579,7 @@
       </c>
       <c r="B2" s="8" t="inlineStr">
         <is>
-          <t>HIGH</t>
+          <t>UNCATEGORIZED</t>
         </is>
       </c>
       <c r="C2" s="8" t="inlineStr">
@@ -3282,7 +3282,7 @@
       </c>
       <c r="B69" s="8" t="inlineStr">
         <is>
-          <t>UNCATEGORIZED</t>
+          <t>HIGH</t>
         </is>
       </c>
       <c r="C69" s="8" t="inlineStr">

</xml_diff>